<commit_message>
cap nhat ngay 4/12/2023
</commit_message>
<xml_diff>
--- a/2023/Demo.xlsx
+++ b/2023/Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trung.nguyenhoang/Documents/github/2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80318AEA-3392-4840-91AD-29DD31B36482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6114083D-9C0E-CF4D-885A-3211C16D5FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17080" xr2:uid="{B7EC2610-802E-D441-AB46-76A27057AA52}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="92">
   <si>
     <t>CHỨNG KHOÁN</t>
   </si>
@@ -183,6 +183,138 @@
   </si>
   <si>
     <t>BÁN LẺ</t>
+  </si>
+  <si>
+    <t>4.07%</t>
+  </si>
+  <si>
+    <t>2.93%</t>
+  </si>
+  <si>
+    <t>18.69%</t>
+  </si>
+  <si>
+    <t>2.66%</t>
+  </si>
+  <si>
+    <t>77.18%</t>
+  </si>
+  <si>
+    <t>1.39%</t>
+  </si>
+  <si>
+    <t>22.51%</t>
+  </si>
+  <si>
+    <t>0.25%</t>
+  </si>
+  <si>
+    <t>13.56%</t>
+  </si>
+  <si>
+    <t>2.00%</t>
+  </si>
+  <si>
+    <t>16.21%</t>
+  </si>
+  <si>
+    <t>2.04%</t>
+  </si>
+  <si>
+    <t>5.67%</t>
+  </si>
+  <si>
+    <t>5.13%</t>
+  </si>
+  <si>
+    <t>34.40%</t>
+  </si>
+  <si>
+    <t>1.19%</t>
+  </si>
+  <si>
+    <t>28.05%</t>
+  </si>
+  <si>
+    <t>1.66%</t>
+  </si>
+  <si>
+    <t>84.19%</t>
+  </si>
+  <si>
+    <t>0.10%</t>
+  </si>
+  <si>
+    <t>50.48%</t>
+  </si>
+  <si>
+    <t>0.84%</t>
+  </si>
+  <si>
+    <t>13.40%</t>
+  </si>
+  <si>
+    <t>2.24%</t>
+  </si>
+  <si>
+    <t>10.84%</t>
+  </si>
+  <si>
+    <t>2.27%</t>
+  </si>
+  <si>
+    <t>2.13%</t>
+  </si>
+  <si>
+    <t>2.46%</t>
+  </si>
+  <si>
+    <t>5.40%</t>
+  </si>
+  <si>
+    <t>2.61%</t>
+  </si>
+  <si>
+    <t>55.07%</t>
+  </si>
+  <si>
+    <t>1.97%</t>
+  </si>
+  <si>
+    <t>4.98%</t>
+  </si>
+  <si>
+    <t>3.24%</t>
+  </si>
+  <si>
+    <t>2.20%</t>
+  </si>
+  <si>
+    <t>4.85%</t>
+  </si>
+  <si>
+    <t>10.39%</t>
+  </si>
+  <si>
+    <t>3.00%</t>
+  </si>
+  <si>
+    <t>2.94%</t>
+  </si>
+  <si>
+    <t>2.70%</t>
+  </si>
+  <si>
+    <t>34.12%</t>
+  </si>
+  <si>
+    <t>1.06%</t>
+  </si>
+  <si>
+    <t>27.16%</t>
+  </si>
+  <si>
+    <t>2.82%</t>
   </si>
 </sst>
 </file>
@@ -380,7 +512,30 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,9 +548,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -405,27 +557,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,11 +908,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9267E568-C429-F945-A885-A15FECEEE65C}">
-  <dimension ref="A1:FU39"/>
+  <dimension ref="A1:FU41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="FS14" sqref="FS14"/>
+      <selection pane="topRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -803,431 +935,431 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
-      <c r="AI1" s="26"/>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="26"/>
-      <c r="AL1" s="26"/>
-      <c r="AM1" s="26"/>
-      <c r="AN1" s="26"/>
-      <c r="AO1" s="27" t="s">
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="27"/>
-      <c r="BB1" s="27"/>
-      <c r="BC1" s="27"/>
+      <c r="AP1" s="16"/>
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="16"/>
+      <c r="AT1" s="16"/>
+      <c r="AU1" s="16"/>
+      <c r="AV1" s="16"/>
+      <c r="AW1" s="16"/>
+      <c r="AX1" s="16"/>
+      <c r="AY1" s="16"/>
+      <c r="AZ1" s="16"/>
+      <c r="BA1" s="16"/>
+      <c r="BB1" s="16"/>
+      <c r="BC1" s="16"/>
       <c r="BD1" s="1"/>
       <c r="BE1" s="1"/>
-      <c r="BF1" s="14" t="s">
+      <c r="BF1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="BG1" s="14"/>
-      <c r="BH1" s="14"/>
-      <c r="BI1" s="14"/>
-      <c r="BJ1" s="14"/>
-      <c r="BK1" s="14"/>
-      <c r="BL1" s="14"/>
-      <c r="BM1" s="14"/>
-      <c r="BN1" s="14"/>
-      <c r="BO1" s="14"/>
-      <c r="BP1" s="14"/>
-      <c r="BQ1" s="14"/>
-      <c r="BR1" s="14"/>
-      <c r="BS1" s="14"/>
-      <c r="BT1" s="14"/>
-      <c r="BU1" s="14"/>
-      <c r="BV1" s="14"/>
-      <c r="BW1" s="14"/>
-      <c r="BX1" s="14"/>
-      <c r="BY1" s="14"/>
-      <c r="BZ1" s="14"/>
-      <c r="CA1" s="14"/>
-      <c r="CB1" s="14"/>
+      <c r="BG1" s="21"/>
+      <c r="BH1" s="21"/>
+      <c r="BI1" s="21"/>
+      <c r="BJ1" s="21"/>
+      <c r="BK1" s="21"/>
+      <c r="BL1" s="21"/>
+      <c r="BM1" s="21"/>
+      <c r="BN1" s="21"/>
+      <c r="BO1" s="21"/>
+      <c r="BP1" s="21"/>
+      <c r="BQ1" s="21"/>
+      <c r="BR1" s="21"/>
+      <c r="BS1" s="21"/>
+      <c r="BT1" s="21"/>
+      <c r="BU1" s="21"/>
+      <c r="BV1" s="21"/>
+      <c r="BW1" s="21"/>
+      <c r="BX1" s="21"/>
+      <c r="BY1" s="21"/>
+      <c r="BZ1" s="21"/>
+      <c r="CA1" s="21"/>
+      <c r="CB1" s="21"/>
       <c r="CC1" s="1"/>
-      <c r="CD1" s="15" t="s">
+      <c r="CD1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="CE1" s="15"/>
-      <c r="CF1" s="15"/>
-      <c r="CG1" s="15"/>
-      <c r="CH1" s="15"/>
-      <c r="CI1" s="15"/>
-      <c r="CJ1" s="15"/>
-      <c r="CK1" s="15"/>
-      <c r="CL1" s="15"/>
-      <c r="CM1" s="15"/>
-      <c r="CN1" s="15"/>
-      <c r="CO1" s="15"/>
-      <c r="CP1" s="15"/>
-      <c r="CQ1" s="15"/>
-      <c r="CR1" s="15"/>
-      <c r="CS1" s="15"/>
-      <c r="CT1" s="15"/>
-      <c r="CU1" s="15"/>
-      <c r="CV1" s="15"/>
-      <c r="CW1" s="15"/>
-      <c r="CX1" s="15"/>
-      <c r="CY1" s="15"/>
-      <c r="CZ1" s="15"/>
-      <c r="DA1" s="15"/>
-      <c r="DB1" s="15"/>
-      <c r="DC1" s="15"/>
-      <c r="DD1" s="15"/>
-      <c r="DE1" s="15"/>
-      <c r="DF1" s="15"/>
-      <c r="DG1" s="15"/>
-      <c r="DH1" s="15"/>
-      <c r="DI1" s="15"/>
-      <c r="DJ1" s="15"/>
-      <c r="DK1" s="15"/>
-      <c r="DL1" s="15"/>
-      <c r="DM1" s="15"/>
-      <c r="DN1" s="15"/>
-      <c r="DO1" s="15"/>
-      <c r="DP1" s="15"/>
+      <c r="CE1" s="22"/>
+      <c r="CF1" s="22"/>
+      <c r="CG1" s="22"/>
+      <c r="CH1" s="22"/>
+      <c r="CI1" s="22"/>
+      <c r="CJ1" s="22"/>
+      <c r="CK1" s="22"/>
+      <c r="CL1" s="22"/>
+      <c r="CM1" s="22"/>
+      <c r="CN1" s="22"/>
+      <c r="CO1" s="22"/>
+      <c r="CP1" s="22"/>
+      <c r="CQ1" s="22"/>
+      <c r="CR1" s="22"/>
+      <c r="CS1" s="22"/>
+      <c r="CT1" s="22"/>
+      <c r="CU1" s="22"/>
+      <c r="CV1" s="22"/>
+      <c r="CW1" s="22"/>
+      <c r="CX1" s="22"/>
+      <c r="CY1" s="22"/>
+      <c r="CZ1" s="22"/>
+      <c r="DA1" s="22"/>
+      <c r="DB1" s="22"/>
+      <c r="DC1" s="22"/>
+      <c r="DD1" s="22"/>
+      <c r="DE1" s="22"/>
+      <c r="DF1" s="22"/>
+      <c r="DG1" s="22"/>
+      <c r="DH1" s="22"/>
+      <c r="DI1" s="22"/>
+      <c r="DJ1" s="22"/>
+      <c r="DK1" s="22"/>
+      <c r="DL1" s="22"/>
+      <c r="DM1" s="22"/>
+      <c r="DN1" s="22"/>
+      <c r="DO1" s="22"/>
+      <c r="DP1" s="22"/>
       <c r="DQ1" s="1"/>
-      <c r="DR1" s="16" t="s">
+      <c r="DR1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="DS1" s="16"/>
-      <c r="DT1" s="16"/>
-      <c r="DU1" s="16"/>
-      <c r="DV1" s="16"/>
-      <c r="DW1" s="16"/>
-      <c r="DX1" s="16"/>
-      <c r="DY1" s="16"/>
-      <c r="DZ1" s="16"/>
-      <c r="EA1" s="16"/>
-      <c r="EB1" s="16"/>
-      <c r="EC1" s="16"/>
-      <c r="ED1" s="16"/>
-      <c r="EE1" s="16"/>
-      <c r="EF1" s="16"/>
+      <c r="DS1" s="23"/>
+      <c r="DT1" s="23"/>
+      <c r="DU1" s="23"/>
+      <c r="DV1" s="23"/>
+      <c r="DW1" s="23"/>
+      <c r="DX1" s="23"/>
+      <c r="DY1" s="23"/>
+      <c r="DZ1" s="23"/>
+      <c r="EA1" s="23"/>
+      <c r="EB1" s="23"/>
+      <c r="EC1" s="23"/>
+      <c r="ED1" s="23"/>
+      <c r="EE1" s="23"/>
+      <c r="EF1" s="23"/>
       <c r="EG1" s="1"/>
-      <c r="EH1" s="23" t="s">
+      <c r="EH1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="EI1" s="23"/>
-      <c r="EJ1" s="23"/>
-      <c r="EK1" s="23"/>
-      <c r="EL1" s="23"/>
-      <c r="EM1" s="23"/>
-      <c r="EN1" s="23"/>
-      <c r="EO1" s="23"/>
-      <c r="EP1" s="23"/>
-      <c r="EQ1" s="23"/>
-      <c r="ER1" s="23"/>
-      <c r="ES1" s="23"/>
-      <c r="ET1" s="23"/>
-      <c r="EU1" s="23"/>
-      <c r="EV1" s="23"/>
+      <c r="EI1" s="19"/>
+      <c r="EJ1" s="19"/>
+      <c r="EK1" s="19"/>
+      <c r="EL1" s="19"/>
+      <c r="EM1" s="19"/>
+      <c r="EN1" s="19"/>
+      <c r="EO1" s="19"/>
+      <c r="EP1" s="19"/>
+      <c r="EQ1" s="19"/>
+      <c r="ER1" s="19"/>
+      <c r="ES1" s="19"/>
+      <c r="ET1" s="19"/>
+      <c r="EU1" s="19"/>
+      <c r="EV1" s="19"/>
       <c r="EW1" s="1"/>
-      <c r="EX1" s="21" t="s">
+      <c r="EX1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="EY1" s="21"/>
-      <c r="EZ1" s="21"/>
-      <c r="FA1" s="21"/>
-      <c r="FB1" s="21"/>
-      <c r="FC1" s="21"/>
-      <c r="FD1" s="21"/>
+      <c r="EY1" s="17"/>
+      <c r="EZ1" s="17"/>
+      <c r="FA1" s="17"/>
+      <c r="FB1" s="17"/>
+      <c r="FC1" s="17"/>
+      <c r="FD1" s="17"/>
       <c r="FE1" s="1"/>
-      <c r="FF1" s="24" t="s">
+      <c r="FF1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="FG1" s="24"/>
-      <c r="FH1" s="24"/>
-      <c r="FI1" s="24"/>
-      <c r="FJ1" s="24"/>
-      <c r="FK1" s="24"/>
-      <c r="FL1" s="24"/>
+      <c r="FG1" s="12"/>
+      <c r="FH1" s="12"/>
+      <c r="FI1" s="12"/>
+      <c r="FJ1" s="12"/>
+      <c r="FK1" s="12"/>
+      <c r="FL1" s="12"/>
       <c r="FM1" s="1"/>
-      <c r="FN1" s="25" t="s">
+      <c r="FN1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="FO1" s="25"/>
-      <c r="FP1" s="25"/>
-      <c r="FQ1" s="25"/>
-      <c r="FR1" s="25"/>
-      <c r="FS1" s="25"/>
-      <c r="FT1" s="25"/>
+      <c r="FO1" s="14"/>
+      <c r="FP1" s="14"/>
+      <c r="FQ1" s="14"/>
+      <c r="FR1" s="14"/>
+      <c r="FS1" s="14"/>
+      <c r="FT1" s="14"/>
       <c r="FU1" s="1"/>
     </row>
     <row r="2" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="22" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="17" t="s">
+      <c r="R2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="17" t="s">
+      <c r="Z2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="17"/>
-      <c r="AC2" s="17"/>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="17"/>
-      <c r="AF2" s="17"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
       <c r="AG2" s="1"/>
-      <c r="AH2" s="17" t="s">
+      <c r="AH2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="AI2" s="17"/>
-      <c r="AJ2" s="17"/>
-      <c r="AK2" s="17"/>
-      <c r="AL2" s="17"/>
-      <c r="AM2" s="17"/>
-      <c r="AN2" s="17"/>
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="13"/>
+      <c r="AK2" s="13"/>
+      <c r="AL2" s="13"/>
+      <c r="AM2" s="13"/>
+      <c r="AN2" s="13"/>
       <c r="AO2" s="1"/>
-      <c r="AP2" s="17" t="s">
+      <c r="AP2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AQ2" s="17"/>
-      <c r="AR2" s="17"/>
-      <c r="AS2" s="17"/>
-      <c r="AT2" s="17"/>
-      <c r="AU2" s="17"/>
-      <c r="AV2" s="17"/>
+      <c r="AQ2" s="13"/>
+      <c r="AR2" s="13"/>
+      <c r="AS2" s="13"/>
+      <c r="AT2" s="13"/>
+      <c r="AU2" s="13"/>
+      <c r="AV2" s="13"/>
       <c r="AW2" s="1"/>
-      <c r="AX2" s="19" t="s">
+      <c r="AX2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="AY2" s="19"/>
-      <c r="AZ2" s="19"/>
-      <c r="BA2" s="19"/>
-      <c r="BB2" s="19"/>
-      <c r="BC2" s="19"/>
-      <c r="BD2" s="20"/>
+      <c r="AY2" s="25"/>
+      <c r="AZ2" s="25"/>
+      <c r="BA2" s="25"/>
+      <c r="BB2" s="25"/>
+      <c r="BC2" s="25"/>
+      <c r="BD2" s="26"/>
       <c r="BE2" s="1"/>
-      <c r="BF2" s="19" t="s">
+      <c r="BF2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="BG2" s="19"/>
-      <c r="BH2" s="19"/>
-      <c r="BI2" s="19"/>
-      <c r="BJ2" s="19"/>
-      <c r="BK2" s="20"/>
+      <c r="BG2" s="25"/>
+      <c r="BH2" s="25"/>
+      <c r="BI2" s="25"/>
+      <c r="BJ2" s="25"/>
+      <c r="BK2" s="26"/>
       <c r="BL2" s="2"/>
       <c r="BM2" s="1"/>
-      <c r="BN2" s="17" t="s">
+      <c r="BN2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="BO2" s="17"/>
-      <c r="BP2" s="17"/>
-      <c r="BQ2" s="17"/>
-      <c r="BR2" s="17"/>
-      <c r="BS2" s="17"/>
-      <c r="BT2" s="17"/>
+      <c r="BO2" s="13"/>
+      <c r="BP2" s="13"/>
+      <c r="BQ2" s="13"/>
+      <c r="BR2" s="13"/>
+      <c r="BS2" s="13"/>
+      <c r="BT2" s="13"/>
       <c r="BU2" s="1"/>
-      <c r="BV2" s="17" t="s">
+      <c r="BV2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="BW2" s="17"/>
-      <c r="BX2" s="17"/>
-      <c r="BY2" s="17"/>
-      <c r="BZ2" s="17"/>
-      <c r="CA2" s="17"/>
-      <c r="CB2" s="17"/>
+      <c r="BW2" s="13"/>
+      <c r="BX2" s="13"/>
+      <c r="BY2" s="13"/>
+      <c r="BZ2" s="13"/>
+      <c r="CA2" s="13"/>
+      <c r="CB2" s="13"/>
       <c r="CC2" s="1"/>
-      <c r="CD2" s="17" t="s">
+      <c r="CD2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="CE2" s="17"/>
-      <c r="CF2" s="17"/>
-      <c r="CG2" s="17"/>
-      <c r="CH2" s="17"/>
-      <c r="CI2" s="17"/>
-      <c r="CJ2" s="17"/>
+      <c r="CE2" s="13"/>
+      <c r="CF2" s="13"/>
+      <c r="CG2" s="13"/>
+      <c r="CH2" s="13"/>
+      <c r="CI2" s="13"/>
+      <c r="CJ2" s="13"/>
       <c r="CK2" s="1"/>
-      <c r="CL2" s="17" t="s">
+      <c r="CL2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="CM2" s="17"/>
-      <c r="CN2" s="17"/>
-      <c r="CO2" s="17"/>
-      <c r="CP2" s="17"/>
-      <c r="CQ2" s="17"/>
-      <c r="CR2" s="17"/>
+      <c r="CM2" s="13"/>
+      <c r="CN2" s="13"/>
+      <c r="CO2" s="13"/>
+      <c r="CP2" s="13"/>
+      <c r="CQ2" s="13"/>
+      <c r="CR2" s="13"/>
       <c r="CS2" s="1"/>
-      <c r="CT2" s="17" t="s">
+      <c r="CT2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="CU2" s="17"/>
-      <c r="CV2" s="17"/>
-      <c r="CW2" s="17"/>
-      <c r="CX2" s="17"/>
-      <c r="CY2" s="17"/>
-      <c r="CZ2" s="17"/>
+      <c r="CU2" s="13"/>
+      <c r="CV2" s="13"/>
+      <c r="CW2" s="13"/>
+      <c r="CX2" s="13"/>
+      <c r="CY2" s="13"/>
+      <c r="CZ2" s="13"/>
       <c r="DA2" s="1"/>
-      <c r="DB2" s="17" t="s">
+      <c r="DB2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="DC2" s="17"/>
-      <c r="DD2" s="17"/>
-      <c r="DE2" s="17"/>
-      <c r="DF2" s="17"/>
-      <c r="DG2" s="17"/>
-      <c r="DH2" s="17"/>
+      <c r="DC2" s="13"/>
+      <c r="DD2" s="13"/>
+      <c r="DE2" s="13"/>
+      <c r="DF2" s="13"/>
+      <c r="DG2" s="13"/>
+      <c r="DH2" s="13"/>
       <c r="DI2" s="1"/>
-      <c r="DJ2" s="17" t="s">
+      <c r="DJ2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="DK2" s="17"/>
-      <c r="DL2" s="17"/>
-      <c r="DM2" s="17"/>
-      <c r="DN2" s="17"/>
-      <c r="DO2" s="17"/>
-      <c r="DP2" s="17"/>
+      <c r="DK2" s="13"/>
+      <c r="DL2" s="13"/>
+      <c r="DM2" s="13"/>
+      <c r="DN2" s="13"/>
+      <c r="DO2" s="13"/>
+      <c r="DP2" s="13"/>
       <c r="DQ2" s="1"/>
-      <c r="DR2" s="17" t="s">
+      <c r="DR2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="DS2" s="17"/>
-      <c r="DT2" s="17"/>
-      <c r="DU2" s="17"/>
-      <c r="DV2" s="17"/>
-      <c r="DW2" s="17"/>
-      <c r="DX2" s="17"/>
+      <c r="DS2" s="13"/>
+      <c r="DT2" s="13"/>
+      <c r="DU2" s="13"/>
+      <c r="DV2" s="13"/>
+      <c r="DW2" s="13"/>
+      <c r="DX2" s="13"/>
       <c r="DY2" s="1"/>
-      <c r="DZ2" s="17" t="s">
+      <c r="DZ2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="EA2" s="17"/>
-      <c r="EB2" s="17"/>
-      <c r="EC2" s="17"/>
-      <c r="ED2" s="17"/>
-      <c r="EE2" s="17"/>
-      <c r="EF2" s="17"/>
+      <c r="EA2" s="13"/>
+      <c r="EB2" s="13"/>
+      <c r="EC2" s="13"/>
+      <c r="ED2" s="13"/>
+      <c r="EE2" s="13"/>
+      <c r="EF2" s="13"/>
       <c r="EG2" s="1"/>
-      <c r="EH2" s="17" t="s">
+      <c r="EH2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="EI2" s="17"/>
-      <c r="EJ2" s="17"/>
-      <c r="EK2" s="17"/>
-      <c r="EL2" s="17"/>
-      <c r="EM2" s="17"/>
-      <c r="EN2" s="17"/>
+      <c r="EI2" s="13"/>
+      <c r="EJ2" s="13"/>
+      <c r="EK2" s="13"/>
+      <c r="EL2" s="13"/>
+      <c r="EM2" s="13"/>
+      <c r="EN2" s="13"/>
       <c r="EO2" s="1"/>
-      <c r="EP2" s="17" t="s">
+      <c r="EP2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="EQ2" s="17"/>
-      <c r="ER2" s="17"/>
-      <c r="ES2" s="17"/>
-      <c r="ET2" s="17"/>
-      <c r="EU2" s="17"/>
-      <c r="EV2" s="17"/>
+      <c r="EQ2" s="13"/>
+      <c r="ER2" s="13"/>
+      <c r="ES2" s="13"/>
+      <c r="ET2" s="13"/>
+      <c r="EU2" s="13"/>
+      <c r="EV2" s="13"/>
       <c r="EW2" s="1"/>
-      <c r="EX2" s="17" t="s">
+      <c r="EX2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="EY2" s="17"/>
-      <c r="EZ2" s="17"/>
-      <c r="FA2" s="17"/>
-      <c r="FB2" s="17"/>
-      <c r="FC2" s="17"/>
-      <c r="FD2" s="17"/>
+      <c r="EY2" s="13"/>
+      <c r="EZ2" s="13"/>
+      <c r="FA2" s="13"/>
+      <c r="FB2" s="13"/>
+      <c r="FC2" s="13"/>
+      <c r="FD2" s="13"/>
       <c r="FE2" s="1"/>
-      <c r="FF2" s="17" t="s">
+      <c r="FF2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="FG2" s="17"/>
-      <c r="FH2" s="17"/>
-      <c r="FI2" s="17"/>
-      <c r="FJ2" s="17"/>
-      <c r="FK2" s="17"/>
-      <c r="FL2" s="17"/>
+      <c r="FG2" s="13"/>
+      <c r="FH2" s="13"/>
+      <c r="FI2" s="13"/>
+      <c r="FJ2" s="13"/>
+      <c r="FK2" s="13"/>
+      <c r="FL2" s="13"/>
       <c r="FM2" s="1"/>
-      <c r="FN2" s="17" t="s">
+      <c r="FN2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="FO2" s="17"/>
-      <c r="FP2" s="17"/>
-      <c r="FQ2" s="17"/>
-      <c r="FR2" s="17"/>
-      <c r="FS2" s="17"/>
-      <c r="FT2" s="17"/>
+      <c r="FO2" s="13"/>
+      <c r="FP2" s="13"/>
+      <c r="FQ2" s="13"/>
+      <c r="FR2" s="13"/>
+      <c r="FS2" s="13"/>
+      <c r="FT2" s="13"/>
       <c r="FU2" s="1"/>
     </row>
     <row r="3" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="11" t="s">
         <v>32</v>
       </c>
@@ -1717,181 +1849,489 @@
       <c r="A4" s="5">
         <v>45245</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
+      <c r="B4" s="6">
+        <v>311300</v>
+      </c>
+      <c r="C4" s="6">
+        <v>629063</v>
+      </c>
+      <c r="D4" s="6">
+        <v>-317763</v>
+      </c>
+      <c r="E4" s="6">
+        <v>-6577320000</v>
+      </c>
+      <c r="F4" s="6">
+        <v>23091100</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="8"/>
+      <c r="J4" s="6">
+        <v>3912700</v>
+      </c>
+      <c r="K4" s="6">
+        <v>1305381</v>
+      </c>
+      <c r="L4" s="6">
+        <v>2607319</v>
+      </c>
+      <c r="M4" s="6">
+        <v>84830510000</v>
+      </c>
+      <c r="N4" s="6">
+        <v>27921501</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="Q4" s="1"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="8"/>
+      <c r="R4" s="6">
+        <v>2028300</v>
+      </c>
+      <c r="S4" s="6">
+        <v>1192340</v>
+      </c>
+      <c r="T4" s="6">
+        <v>835960</v>
+      </c>
+      <c r="U4" s="6">
+        <v>72420650000</v>
+      </c>
+      <c r="V4" s="6">
+        <v>4172800</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="X4" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="7"/>
-      <c r="AF4" s="8"/>
+      <c r="Z4" s="6">
+        <v>1897100</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>2139200</v>
+      </c>
+      <c r="AB4" s="6">
+        <v>-242100</v>
+      </c>
+      <c r="AC4" s="6">
+        <v>-4833120000</v>
+      </c>
+      <c r="AD4" s="6">
+        <v>17930900</v>
+      </c>
+      <c r="AE4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF4" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="AG4" s="1"/>
-      <c r="AH4" s="6"/>
-      <c r="AI4" s="6"/>
-      <c r="AJ4" s="6"/>
-      <c r="AK4" s="6"/>
-      <c r="AL4" s="6"/>
-      <c r="AM4" s="7"/>
-      <c r="AN4" s="8"/>
+      <c r="AH4" s="6">
+        <v>683000</v>
+      </c>
+      <c r="AI4" s="6">
+        <v>2430533</v>
+      </c>
+      <c r="AJ4" s="6">
+        <v>-1747533</v>
+      </c>
+      <c r="AK4" s="6">
+        <v>-52841490000</v>
+      </c>
+      <c r="AL4" s="6">
+        <v>22967100</v>
+      </c>
+      <c r="AM4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN4" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="AO4" s="1"/>
-      <c r="AP4" s="6"/>
-      <c r="AQ4" s="6"/>
-      <c r="AR4" s="6"/>
-      <c r="AS4" s="6"/>
-      <c r="AT4" s="6"/>
-      <c r="AU4" s="7"/>
-      <c r="AV4" s="8"/>
+      <c r="AP4" s="6">
+        <v>3242900</v>
+      </c>
+      <c r="AQ4" s="6">
+        <v>2395611</v>
+      </c>
+      <c r="AR4" s="6">
+        <v>847289</v>
+      </c>
+      <c r="AS4" s="6">
+        <v>23110240000</v>
+      </c>
+      <c r="AT4" s="6">
+        <v>34793000</v>
+      </c>
+      <c r="AU4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV4" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="AW4" s="1"/>
-      <c r="AX4" s="6"/>
-      <c r="AY4" s="6"/>
-      <c r="AZ4" s="6"/>
-      <c r="BA4" s="6"/>
-      <c r="BB4" s="6"/>
-      <c r="BC4" s="7"/>
-      <c r="BD4" s="8"/>
+      <c r="AX4" s="6">
+        <v>592400</v>
+      </c>
+      <c r="AY4" s="6">
+        <v>375300</v>
+      </c>
+      <c r="AZ4" s="6">
+        <v>217100</v>
+      </c>
+      <c r="BA4" s="6">
+        <v>4567720000</v>
+      </c>
+      <c r="BB4" s="6">
+        <v>17054000</v>
+      </c>
+      <c r="BC4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD4" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="BE4" s="1"/>
-      <c r="BF4" s="6"/>
-      <c r="BG4" s="6"/>
-      <c r="BH4" s="6"/>
-      <c r="BI4" s="6"/>
-      <c r="BJ4" s="6"/>
-      <c r="BK4" s="7"/>
-      <c r="BL4" s="8"/>
+      <c r="BF4" s="6">
+        <v>1744700</v>
+      </c>
+      <c r="BG4" s="6">
+        <v>2690000</v>
+      </c>
+      <c r="BH4" s="6">
+        <v>-945300</v>
+      </c>
+      <c r="BI4" s="6">
+        <v>-40044580000</v>
+      </c>
+      <c r="BJ4" s="6">
+        <v>12890300</v>
+      </c>
+      <c r="BK4" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL4" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="BM4" s="1"/>
-      <c r="BN4" s="6"/>
-      <c r="BO4" s="6"/>
-      <c r="BP4" s="6"/>
-      <c r="BQ4" s="6"/>
-      <c r="BR4" s="6"/>
-      <c r="BS4" s="7"/>
-      <c r="BT4" s="8"/>
+      <c r="BN4" s="6">
+        <v>566200</v>
+      </c>
+      <c r="BO4" s="6">
+        <v>539661</v>
+      </c>
+      <c r="BP4" s="6">
+        <v>26539</v>
+      </c>
+      <c r="BQ4" s="6">
+        <v>741340000</v>
+      </c>
+      <c r="BR4" s="6">
+        <v>3942600</v>
+      </c>
+      <c r="BS4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="BT4" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="BU4" s="1"/>
-      <c r="BV4" s="6"/>
-      <c r="BW4" s="6"/>
-      <c r="BX4" s="6"/>
-      <c r="BY4" s="6"/>
-      <c r="BZ4" s="6"/>
-      <c r="CA4" s="7"/>
-      <c r="CB4" s="8"/>
+      <c r="BV4" s="6">
+        <v>279000</v>
+      </c>
+      <c r="BW4" s="6">
+        <v>134200</v>
+      </c>
+      <c r="BX4" s="6">
+        <v>144800</v>
+      </c>
+      <c r="BY4" s="6">
+        <v>15098420000</v>
+      </c>
+      <c r="BZ4" s="6">
+        <v>490800</v>
+      </c>
+      <c r="CA4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="CB4" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="CC4" s="1"/>
-      <c r="CD4" s="6"/>
-      <c r="CE4" s="6"/>
-      <c r="CF4" s="6"/>
-      <c r="CG4" s="6"/>
-      <c r="CH4" s="6"/>
-      <c r="CI4" s="7"/>
-      <c r="CJ4" s="8"/>
+      <c r="CD4" s="6">
+        <v>1483500</v>
+      </c>
+      <c r="CE4" s="6">
+        <v>2850444</v>
+      </c>
+      <c r="CF4" s="6">
+        <v>-1366944</v>
+      </c>
+      <c r="CG4" s="6">
+        <v>-57178000000</v>
+      </c>
+      <c r="CH4" s="6">
+        <v>8585400</v>
+      </c>
+      <c r="CI4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="CJ4" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="CK4" s="1"/>
-      <c r="CL4" s="6"/>
-      <c r="CM4" s="6"/>
-      <c r="CN4" s="6"/>
-      <c r="CO4" s="6"/>
-      <c r="CP4" s="6"/>
-      <c r="CQ4" s="7"/>
-      <c r="CR4" s="8"/>
+      <c r="CL4" s="6">
+        <v>2925000</v>
+      </c>
+      <c r="CM4" s="6">
+        <v>268607</v>
+      </c>
+      <c r="CN4" s="6">
+        <v>2656393</v>
+      </c>
+      <c r="CO4" s="6">
+        <v>53611410000</v>
+      </c>
+      <c r="CP4" s="6">
+        <v>23838600</v>
+      </c>
+      <c r="CQ4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="CR4" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="CS4" s="1"/>
-      <c r="CT4" s="6"/>
-      <c r="CU4" s="6"/>
-      <c r="CV4" s="6"/>
-      <c r="CW4" s="6"/>
-      <c r="CX4" s="6"/>
-      <c r="CY4" s="7"/>
-      <c r="CZ4" s="8"/>
+      <c r="CT4" s="6">
+        <v>1439100</v>
+      </c>
+      <c r="CU4" s="6">
+        <v>535700</v>
+      </c>
+      <c r="CV4" s="6">
+        <v>903400</v>
+      </c>
+      <c r="CW4" s="6">
+        <v>24475880000</v>
+      </c>
+      <c r="CX4" s="6">
+        <v>18214600</v>
+      </c>
+      <c r="CY4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="CZ4" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="DA4" s="1"/>
-      <c r="DB4" s="6"/>
-      <c r="DC4" s="6"/>
-      <c r="DD4" s="6"/>
-      <c r="DE4" s="6"/>
-      <c r="DF4" s="6"/>
-      <c r="DG4" s="7"/>
-      <c r="DH4" s="8"/>
+      <c r="DB4" s="6">
+        <v>50700</v>
+      </c>
+      <c r="DC4" s="6">
+        <v>590304</v>
+      </c>
+      <c r="DD4" s="6">
+        <v>-539604</v>
+      </c>
+      <c r="DE4" s="6">
+        <v>-8902670000</v>
+      </c>
+      <c r="DF4" s="6">
+        <v>30081700</v>
+      </c>
+      <c r="DG4" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="DH4" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="DI4" s="1"/>
-      <c r="DJ4" s="6"/>
-      <c r="DK4" s="6"/>
-      <c r="DL4" s="6"/>
-      <c r="DM4" s="6"/>
-      <c r="DN4" s="6"/>
-      <c r="DO4" s="7"/>
-      <c r="DP4" s="8"/>
+      <c r="DJ4" s="6">
+        <v>106600</v>
+      </c>
+      <c r="DK4" s="6">
+        <v>297400</v>
+      </c>
+      <c r="DL4" s="6">
+        <v>-190800</v>
+      </c>
+      <c r="DM4" s="6">
+        <v>-5900820000</v>
+      </c>
+      <c r="DN4" s="6">
+        <v>7475400</v>
+      </c>
+      <c r="DO4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="DP4" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="DQ4" s="1"/>
-      <c r="DR4" s="6"/>
-      <c r="DS4" s="6"/>
-      <c r="DT4" s="6"/>
-      <c r="DU4" s="6"/>
-      <c r="DV4" s="6"/>
-      <c r="DW4" s="7"/>
-      <c r="DX4" s="8"/>
+      <c r="DR4" s="6">
+        <v>237510</v>
+      </c>
+      <c r="DS4" s="6">
+        <v>310600</v>
+      </c>
+      <c r="DT4" s="6">
+        <v>-73090</v>
+      </c>
+      <c r="DU4" s="6">
+        <v>-4972470000</v>
+      </c>
+      <c r="DV4" s="6">
+        <v>995300</v>
+      </c>
+      <c r="DW4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="DX4" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="DY4" s="1"/>
-      <c r="DZ4" s="6"/>
-      <c r="EA4" s="6"/>
-      <c r="EB4" s="6"/>
-      <c r="EC4" s="6"/>
-      <c r="ED4" s="6"/>
-      <c r="EE4" s="7"/>
-      <c r="EF4" s="8"/>
+      <c r="DZ4" s="6">
+        <v>3000</v>
+      </c>
+      <c r="EA4" s="6">
+        <v>108300</v>
+      </c>
+      <c r="EB4" s="6">
+        <v>-105300</v>
+      </c>
+      <c r="EC4" s="6">
+        <v>-3638730000</v>
+      </c>
+      <c r="ED4" s="6">
+        <v>2234600</v>
+      </c>
+      <c r="EE4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="EF4" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="EG4" s="1"/>
-      <c r="EH4" s="6"/>
-      <c r="EI4" s="6"/>
-      <c r="EJ4" s="6"/>
-      <c r="EK4" s="6"/>
-      <c r="EL4" s="6"/>
-      <c r="EM4" s="7"/>
-      <c r="EN4" s="8"/>
+      <c r="EH4" s="6">
+        <v>8100</v>
+      </c>
+      <c r="EI4" s="6">
+        <v>72817</v>
+      </c>
+      <c r="EJ4" s="6">
+        <v>-64717</v>
+      </c>
+      <c r="EK4" s="6">
+        <v>-4086470000</v>
+      </c>
+      <c r="EL4" s="6">
+        <v>3684500</v>
+      </c>
+      <c r="EM4" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="EN4" s="8" t="s">
+        <v>83</v>
+      </c>
       <c r="EO4" s="1"/>
-      <c r="EP4" s="6"/>
-      <c r="EQ4" s="6"/>
-      <c r="ER4" s="6"/>
-      <c r="ES4" s="6"/>
-      <c r="ET4" s="6"/>
-      <c r="EU4" s="7"/>
-      <c r="EV4" s="8"/>
+      <c r="EP4" s="6">
+        <v>321000</v>
+      </c>
+      <c r="EQ4" s="6">
+        <v>481300</v>
+      </c>
+      <c r="ER4" s="6">
+        <v>-160300</v>
+      </c>
+      <c r="ES4" s="6">
+        <v>-3829830000</v>
+      </c>
+      <c r="ET4" s="6">
+        <v>7719200</v>
+      </c>
+      <c r="EU4" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="EV4" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="EW4" s="1"/>
-      <c r="EX4" s="6"/>
-      <c r="EY4" s="6"/>
-      <c r="EZ4" s="6"/>
-      <c r="FA4" s="6"/>
-      <c r="FB4" s="6"/>
-      <c r="FC4" s="7"/>
-      <c r="FD4" s="8"/>
+      <c r="EX4" s="6">
+        <v>53300</v>
+      </c>
+      <c r="EY4" s="6">
+        <v>498500</v>
+      </c>
+      <c r="EZ4" s="6">
+        <v>-445200</v>
+      </c>
+      <c r="FA4" s="6">
+        <v>-9980060000</v>
+      </c>
+      <c r="FB4" s="6">
+        <v>18792600</v>
+      </c>
+      <c r="FC4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="FD4" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="FE4" s="1"/>
-      <c r="FF4" s="6"/>
-      <c r="FG4" s="6"/>
-      <c r="FH4" s="6"/>
-      <c r="FI4" s="6"/>
-      <c r="FJ4" s="6"/>
-      <c r="FK4" s="7"/>
-      <c r="FL4" s="8"/>
+      <c r="FF4" s="6">
+        <v>626600</v>
+      </c>
+      <c r="FG4" s="6">
+        <v>142510</v>
+      </c>
+      <c r="FH4" s="6">
+        <v>484090</v>
+      </c>
+      <c r="FI4" s="6">
+        <v>45728080000</v>
+      </c>
+      <c r="FJ4" s="6">
+        <v>2254400</v>
+      </c>
+      <c r="FK4" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="FL4" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="FM4" s="1"/>
-      <c r="FN4" s="6"/>
-      <c r="FO4" s="6"/>
-      <c r="FP4" s="6"/>
-      <c r="FQ4" s="6"/>
-      <c r="FR4" s="6"/>
-      <c r="FS4" s="7"/>
-      <c r="FT4" s="8"/>
+      <c r="FN4" s="6">
+        <v>220100</v>
+      </c>
+      <c r="FO4" s="6">
+        <v>166000</v>
+      </c>
+      <c r="FP4" s="6">
+        <v>54100</v>
+      </c>
+      <c r="FQ4" s="6">
+        <v>3878960000</v>
+      </c>
+      <c r="FR4" s="6">
+        <v>1421800</v>
+      </c>
+      <c r="FS4" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="FT4" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="FU4" s="1"/>
     </row>
     <row r="5" spans="1:177" x14ac:dyDescent="0.2">
@@ -2258,15 +2698,15 @@
     </row>
     <row r="7" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
-        <v>45250</v>
-      </c>
-      <c r="B7" s="6"/>
+        <v>45248</v>
+      </c>
+      <c r="B7" s="7"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="1"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -2396,7 +2836,6 @@
       <c r="EE7" s="7"/>
       <c r="EF7" s="8"/>
       <c r="EG7" s="1"/>
-      <c r="EH7" s="6"/>
       <c r="EI7" s="6"/>
       <c r="EJ7" s="6"/>
       <c r="EK7" s="6"/>
@@ -2439,7 +2878,7 @@
     </row>
     <row r="8" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
-        <v>45251</v>
+        <v>45249</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2620,7 +3059,7 @@
     </row>
     <row r="9" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
-        <v>45252</v>
+        <v>45250</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2679,12 +3118,12 @@
       <c r="BD9" s="8"/>
       <c r="BE9" s="1"/>
       <c r="BF9" s="6"/>
-      <c r="BG9" s="7"/>
-      <c r="BH9" s="7"/>
+      <c r="BG9" s="6"/>
+      <c r="BH9" s="6"/>
       <c r="BI9" s="6"/>
       <c r="BJ9" s="6"/>
       <c r="BK9" s="7"/>
-      <c r="BL9" s="7"/>
+      <c r="BL9" s="8"/>
       <c r="BM9" s="1"/>
       <c r="BN9" s="6"/>
       <c r="BO9" s="6"/>
@@ -2801,7 +3240,7 @@
     </row>
     <row r="10" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
-        <v>45253</v>
+        <v>45251</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -2982,7 +3421,7 @@
     </row>
     <row r="11" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
-        <v>45254</v>
+        <v>45252</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -3041,12 +3480,12 @@
       <c r="BD11" s="8"/>
       <c r="BE11" s="1"/>
       <c r="BF11" s="6"/>
-      <c r="BG11" s="6"/>
-      <c r="BH11" s="6"/>
+      <c r="BG11" s="7"/>
+      <c r="BH11" s="7"/>
       <c r="BI11" s="6"/>
       <c r="BJ11" s="6"/>
       <c r="BK11" s="7"/>
-      <c r="BL11" s="8"/>
+      <c r="BL11" s="7"/>
       <c r="BM11" s="1"/>
       <c r="BN11" s="6"/>
       <c r="BO11" s="6"/>
@@ -3163,7 +3602,7 @@
     </row>
     <row r="12" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
-        <v>45257</v>
+        <v>45253</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -3344,7 +3783,7 @@
     </row>
     <row r="13" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
-        <v>45258</v>
+        <v>45254</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -3525,7 +3964,7 @@
     </row>
     <row r="14" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
-        <v>45259</v>
+        <v>45257</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -3569,6 +4008,7 @@
       <c r="AO14" s="1"/>
       <c r="AP14" s="6"/>
       <c r="AQ14" s="6"/>
+      <c r="AR14" s="6"/>
       <c r="AS14" s="6"/>
       <c r="AT14" s="6"/>
       <c r="AU14" s="7"/>
@@ -3705,7 +4145,7 @@
     </row>
     <row r="15" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
-        <v>45260</v>
+        <v>45258</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -3886,7 +4326,7 @@
     </row>
     <row r="16" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
-        <v>45261</v>
+        <v>45259</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -3930,7 +4370,6 @@
       <c r="AO16" s="1"/>
       <c r="AP16" s="6"/>
       <c r="AQ16" s="6"/>
-      <c r="AR16" s="6"/>
       <c r="AS16" s="6"/>
       <c r="AT16" s="6"/>
       <c r="AU16" s="7"/>
@@ -4067,33 +4506,53 @@
     </row>
     <row r="17" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
-        <v>45264</v>
-      </c>
+        <v>45260</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="7"/>
       <c r="H17" s="8"/>
       <c r="I17" s="1"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
       <c r="O17" s="7"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="1"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
       <c r="W17" s="7"/>
       <c r="X17" s="8"/>
       <c r="Y17" s="1"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
       <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
       <c r="AE17" s="7"/>
       <c r="AF17" s="8"/>
       <c r="AG17" s="1"/>
+      <c r="AH17" s="6"/>
+      <c r="AI17" s="6"/>
       <c r="AJ17" s="6"/>
       <c r="AK17" s="6"/>
+      <c r="AL17" s="6"/>
       <c r="AM17" s="7"/>
       <c r="AN17" s="8"/>
       <c r="AO17" s="1"/>
+      <c r="AP17" s="6"/>
+      <c r="AQ17" s="6"/>
       <c r="AR17" s="6"/>
       <c r="AS17" s="6"/>
+      <c r="AT17" s="6"/>
       <c r="AU17" s="7"/>
       <c r="AV17" s="8"/>
       <c r="AW17" s="1"/>
@@ -4105,111 +4564,176 @@
       <c r="BC17" s="7"/>
       <c r="BD17" s="8"/>
       <c r="BE17" s="1"/>
+      <c r="BF17" s="6"/>
+      <c r="BG17" s="6"/>
       <c r="BH17" s="6"/>
       <c r="BI17" s="6"/>
+      <c r="BJ17" s="6"/>
       <c r="BK17" s="7"/>
       <c r="BL17" s="8"/>
       <c r="BM17" s="1"/>
+      <c r="BN17" s="6"/>
+      <c r="BO17" s="6"/>
       <c r="BP17" s="6"/>
       <c r="BQ17" s="6"/>
+      <c r="BR17" s="6"/>
       <c r="BS17" s="7"/>
       <c r="BT17" s="8"/>
       <c r="BU17" s="1"/>
+      <c r="BV17" s="6"/>
+      <c r="BW17" s="6"/>
       <c r="BX17" s="6"/>
       <c r="BY17" s="6"/>
+      <c r="BZ17" s="6"/>
       <c r="CA17" s="7"/>
       <c r="CB17" s="8"/>
       <c r="CC17" s="1"/>
+      <c r="CD17" s="6"/>
+      <c r="CE17" s="6"/>
       <c r="CF17" s="6"/>
       <c r="CG17" s="6"/>
+      <c r="CH17" s="6"/>
       <c r="CI17" s="7"/>
       <c r="CJ17" s="8"/>
       <c r="CK17" s="1"/>
+      <c r="CL17" s="6"/>
+      <c r="CM17" s="6"/>
       <c r="CN17" s="6"/>
       <c r="CO17" s="6"/>
+      <c r="CP17" s="6"/>
       <c r="CQ17" s="7"/>
       <c r="CR17" s="8"/>
       <c r="CS17" s="1"/>
+      <c r="CT17" s="6"/>
+      <c r="CU17" s="6"/>
       <c r="CV17" s="6"/>
       <c r="CW17" s="6"/>
+      <c r="CX17" s="6"/>
       <c r="CY17" s="7"/>
       <c r="CZ17" s="8"/>
       <c r="DA17" s="1"/>
+      <c r="DB17" s="6"/>
+      <c r="DC17" s="6"/>
       <c r="DD17" s="6"/>
       <c r="DE17" s="6"/>
+      <c r="DF17" s="6"/>
       <c r="DG17" s="7"/>
       <c r="DH17" s="8"/>
       <c r="DI17" s="1"/>
+      <c r="DJ17" s="6"/>
+      <c r="DK17" s="6"/>
       <c r="DL17" s="6"/>
       <c r="DM17" s="6"/>
+      <c r="DN17" s="6"/>
       <c r="DO17" s="7"/>
       <c r="DP17" s="8"/>
       <c r="DQ17" s="1"/>
+      <c r="DR17" s="6"/>
+      <c r="DS17" s="6"/>
       <c r="DT17" s="6"/>
       <c r="DU17" s="6"/>
+      <c r="DV17" s="6"/>
       <c r="DW17" s="7"/>
       <c r="DX17" s="8"/>
       <c r="DY17" s="1"/>
+      <c r="DZ17" s="6"/>
+      <c r="EA17" s="6"/>
       <c r="EB17" s="6"/>
       <c r="EC17" s="6"/>
+      <c r="ED17" s="6"/>
       <c r="EE17" s="7"/>
       <c r="EF17" s="8"/>
       <c r="EG17" s="1"/>
+      <c r="EH17" s="6"/>
+      <c r="EI17" s="6"/>
       <c r="EJ17" s="6"/>
       <c r="EK17" s="6"/>
+      <c r="EL17" s="6"/>
       <c r="EM17" s="7"/>
       <c r="EN17" s="8"/>
       <c r="EO17" s="1"/>
+      <c r="EP17" s="6"/>
+      <c r="EQ17" s="6"/>
       <c r="ER17" s="6"/>
       <c r="ES17" s="6"/>
+      <c r="ET17" s="6"/>
       <c r="EU17" s="7"/>
       <c r="EV17" s="8"/>
       <c r="EW17" s="1"/>
+      <c r="EX17" s="6"/>
+      <c r="EY17" s="6"/>
       <c r="EZ17" s="6"/>
       <c r="FA17" s="6"/>
+      <c r="FB17" s="6"/>
       <c r="FC17" s="7"/>
       <c r="FD17" s="8"/>
       <c r="FE17" s="1"/>
+      <c r="FF17" s="6"/>
+      <c r="FG17" s="6"/>
       <c r="FH17" s="6"/>
       <c r="FI17" s="6"/>
+      <c r="FJ17" s="6"/>
       <c r="FK17" s="7"/>
       <c r="FL17" s="8"/>
       <c r="FM17" s="1"/>
+      <c r="FN17" s="6"/>
+      <c r="FO17" s="6"/>
       <c r="FP17" s="6"/>
       <c r="FQ17" s="6"/>
+      <c r="FR17" s="6"/>
       <c r="FS17" s="7"/>
       <c r="FT17" s="8"/>
       <c r="FU17" s="1"/>
     </row>
     <row r="18" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
-        <v>45265</v>
-      </c>
+        <v>45261</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="7"/>
       <c r="H18" s="8"/>
       <c r="I18" s="1"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
       <c r="O18" s="7"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="1"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
       <c r="W18" s="7"/>
       <c r="X18" s="8"/>
       <c r="Y18" s="1"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
       <c r="AC18" s="6"/>
+      <c r="AD18" s="6"/>
       <c r="AE18" s="7"/>
       <c r="AF18" s="8"/>
       <c r="AG18" s="1"/>
+      <c r="AH18" s="6"/>
+      <c r="AI18" s="6"/>
       <c r="AJ18" s="6"/>
       <c r="AK18" s="6"/>
+      <c r="AL18" s="6"/>
       <c r="AM18" s="7"/>
       <c r="AN18" s="8"/>
       <c r="AO18" s="1"/>
+      <c r="AP18" s="6"/>
+      <c r="AQ18" s="6"/>
       <c r="AR18" s="6"/>
       <c r="AS18" s="6"/>
+      <c r="AT18" s="6"/>
       <c r="AU18" s="7"/>
       <c r="AV18" s="8"/>
       <c r="AW18" s="1"/>
@@ -4221,85 +4745,130 @@
       <c r="BC18" s="7"/>
       <c r="BD18" s="8"/>
       <c r="BE18" s="1"/>
+      <c r="BF18" s="6"/>
+      <c r="BG18" s="6"/>
       <c r="BH18" s="6"/>
       <c r="BI18" s="6"/>
+      <c r="BJ18" s="6"/>
       <c r="BK18" s="7"/>
       <c r="BL18" s="8"/>
       <c r="BM18" s="1"/>
+      <c r="BN18" s="6"/>
+      <c r="BO18" s="6"/>
       <c r="BP18" s="6"/>
       <c r="BQ18" s="6"/>
+      <c r="BR18" s="6"/>
       <c r="BS18" s="7"/>
       <c r="BT18" s="8"/>
       <c r="BU18" s="1"/>
+      <c r="BV18" s="6"/>
+      <c r="BW18" s="6"/>
       <c r="BX18" s="6"/>
       <c r="BY18" s="6"/>
+      <c r="BZ18" s="6"/>
       <c r="CA18" s="7"/>
       <c r="CB18" s="8"/>
       <c r="CC18" s="1"/>
+      <c r="CD18" s="6"/>
+      <c r="CE18" s="6"/>
       <c r="CF18" s="6"/>
       <c r="CG18" s="6"/>
+      <c r="CH18" s="6"/>
       <c r="CI18" s="7"/>
       <c r="CJ18" s="8"/>
       <c r="CK18" s="1"/>
+      <c r="CL18" s="6"/>
+      <c r="CM18" s="6"/>
       <c r="CN18" s="6"/>
       <c r="CO18" s="6"/>
+      <c r="CP18" s="6"/>
       <c r="CQ18" s="7"/>
       <c r="CR18" s="8"/>
       <c r="CS18" s="1"/>
+      <c r="CT18" s="6"/>
+      <c r="CU18" s="6"/>
       <c r="CV18" s="6"/>
       <c r="CW18" s="6"/>
+      <c r="CX18" s="6"/>
       <c r="CY18" s="7"/>
       <c r="CZ18" s="8"/>
       <c r="DA18" s="1"/>
+      <c r="DB18" s="6"/>
+      <c r="DC18" s="6"/>
       <c r="DD18" s="6"/>
       <c r="DE18" s="6"/>
+      <c r="DF18" s="6"/>
       <c r="DG18" s="7"/>
       <c r="DH18" s="8"/>
       <c r="DI18" s="1"/>
+      <c r="DJ18" s="6"/>
+      <c r="DK18" s="6"/>
       <c r="DL18" s="6"/>
       <c r="DM18" s="6"/>
+      <c r="DN18" s="6"/>
       <c r="DO18" s="7"/>
       <c r="DP18" s="8"/>
       <c r="DQ18" s="1"/>
+      <c r="DR18" s="6"/>
+      <c r="DS18" s="6"/>
       <c r="DT18" s="6"/>
       <c r="DU18" s="6"/>
+      <c r="DV18" s="6"/>
       <c r="DW18" s="7"/>
       <c r="DX18" s="8"/>
       <c r="DY18" s="1"/>
+      <c r="DZ18" s="6"/>
+      <c r="EA18" s="6"/>
       <c r="EB18" s="6"/>
       <c r="EC18" s="6"/>
+      <c r="ED18" s="6"/>
       <c r="EE18" s="7"/>
       <c r="EF18" s="8"/>
       <c r="EG18" s="1"/>
+      <c r="EH18" s="6"/>
+      <c r="EI18" s="6"/>
       <c r="EJ18" s="6"/>
       <c r="EK18" s="6"/>
+      <c r="EL18" s="6"/>
       <c r="EM18" s="7"/>
       <c r="EN18" s="8"/>
       <c r="EO18" s="1"/>
+      <c r="EP18" s="6"/>
+      <c r="EQ18" s="6"/>
       <c r="ER18" s="6"/>
       <c r="ES18" s="6"/>
+      <c r="ET18" s="6"/>
       <c r="EU18" s="7"/>
       <c r="EV18" s="8"/>
       <c r="EW18" s="1"/>
+      <c r="EX18" s="6"/>
+      <c r="EY18" s="6"/>
       <c r="EZ18" s="6"/>
       <c r="FA18" s="6"/>
+      <c r="FB18" s="6"/>
       <c r="FC18" s="7"/>
       <c r="FD18" s="8"/>
       <c r="FE18" s="1"/>
+      <c r="FF18" s="6"/>
+      <c r="FG18" s="6"/>
       <c r="FH18" s="6"/>
       <c r="FI18" s="6"/>
+      <c r="FJ18" s="6"/>
       <c r="FK18" s="7"/>
       <c r="FL18" s="8"/>
       <c r="FM18" s="1"/>
+      <c r="FN18" s="6"/>
+      <c r="FO18" s="6"/>
       <c r="FP18" s="6"/>
       <c r="FQ18" s="6"/>
+      <c r="FR18" s="6"/>
       <c r="FS18" s="7"/>
       <c r="FT18" s="8"/>
       <c r="FU18" s="1"/>
     </row>
     <row r="19" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
-        <v>45266</v>
+        <v>45264</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="8"/>
@@ -4415,7 +4984,7 @@
     </row>
     <row r="20" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
-        <v>45267</v>
+        <v>45265</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="8"/>
@@ -4531,7 +5100,7 @@
     </row>
     <row r="21" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
-        <v>45268</v>
+        <v>45266</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="8"/>
@@ -4647,7 +5216,7 @@
     </row>
     <row r="22" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
-        <v>45271</v>
+        <v>45267</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="8"/>
@@ -4763,7 +5332,7 @@
     </row>
     <row r="23" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
-        <v>45272</v>
+        <v>45268</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="8"/>
@@ -4879,7 +5448,7 @@
     </row>
     <row r="24" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
-        <v>45273</v>
+        <v>45271</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="8"/>
@@ -4995,7 +5564,7 @@
     </row>
     <row r="25" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
-        <v>45274</v>
+        <v>45272</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="8"/>
@@ -5111,14 +5680,13 @@
     </row>
     <row r="26" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
-        <v>45275</v>
+        <v>45273</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="8"/>
       <c r="I26" s="1"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
       <c r="O26" s="7"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="1"/>
@@ -5227,13 +5795,14 @@
       <c r="FU26" s="1"/>
     </row>
     <row r="27" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
+      <c r="A27" s="5">
+        <v>45274</v>
+      </c>
       <c r="G27" s="7"/>
       <c r="H27" s="8"/>
       <c r="I27" s="1"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
       <c r="O27" s="7"/>
       <c r="P27" s="8"/>
       <c r="Q27" s="1"/>
@@ -5342,879 +5911,1128 @@
       <c r="FU27" s="1"/>
     </row>
     <row r="28" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="12" t="e">
-        <f>AVERAGE(B4:B25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C28" s="6" t="e">
-        <f>AVERAGE(C4:C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F28" s="6" t="e">
-        <f>AVERAGE(F4:F25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G28" s="6"/>
+      <c r="A28" s="5">
+        <v>45275</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="8"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="6" t="e">
-        <f>AVERAGE(J4:J25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N28" s="6" t="e">
-        <f>AVERAGE(N4:N25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="8"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="6" t="e">
-        <f>AVERAGE(R4:R26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S28" s="6" t="e">
-        <f>AVERAGE(S4:S26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V28" s="6" t="e">
-        <f>AVERAGE(V4:V25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="8"/>
       <c r="Y28" s="1"/>
-      <c r="Z28" s="6" t="e">
-        <f>AVERAGE(Z4:Z26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA28" s="6" t="e">
-        <f>AVERAGE(AA4:AA25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD28" s="6" t="e">
-        <f>AVERAGE(AD4:AD25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AB28" s="6"/>
+      <c r="AC28" s="6"/>
+      <c r="AE28" s="7"/>
+      <c r="AF28" s="8"/>
       <c r="AG28" s="1"/>
-      <c r="AH28" s="6" t="e">
-        <f>AVERAGE(AH4:AH26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI28" s="6" t="e">
-        <f>AVERAGE(AI4:AI25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AL28" s="6" t="e">
-        <f>AVERAGE(AL4:AL25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ28" s="6"/>
+      <c r="AK28" s="6"/>
+      <c r="AM28" s="7"/>
+      <c r="AN28" s="8"/>
       <c r="AO28" s="1"/>
-      <c r="AP28" s="6" t="e">
-        <f>AVERAGE(AP4:AP26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AQ28" s="6" t="e">
-        <f>AVERAGE(AQ4:AQ25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AT28" s="6" t="e">
-        <f>AVERAGE(AT4:AT25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AR28" s="6"/>
+      <c r="AS28" s="6"/>
+      <c r="AU28" s="7"/>
+      <c r="AV28" s="8"/>
       <c r="AW28" s="1"/>
-      <c r="AX28" s="6" t="e">
-        <f>AVERAGE(AX4:AX26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AY28" s="6" t="e">
-        <f>AVERAGE(AY4:AY25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BB28" s="6" t="e">
-        <f>AVERAGE(BB4:BB25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AX28" s="6"/>
+      <c r="AY28" s="6"/>
+      <c r="AZ28" s="6"/>
+      <c r="BA28" s="6"/>
+      <c r="BB28" s="6"/>
+      <c r="BC28" s="7"/>
+      <c r="BD28" s="8"/>
       <c r="BE28" s="1"/>
-      <c r="BF28" s="6" t="e">
-        <f>AVERAGE(BF4:BF26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BG28" s="6" t="e">
-        <f>AVERAGE(BG4:BG25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BJ28" s="6" t="e">
-        <f>AVERAGE(BJ4:BJ25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="BH28" s="6"/>
+      <c r="BI28" s="6"/>
+      <c r="BK28" s="7"/>
+      <c r="BL28" s="8"/>
       <c r="BM28" s="1"/>
-      <c r="BN28" s="6" t="e">
-        <f>AVERAGE(BN4:BN26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BO28" s="6" t="e">
-        <f>AVERAGE(BO4:BO25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BR28" s="6" t="e">
-        <f>AVERAGE(BR4:BR25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="BP28" s="6"/>
+      <c r="BQ28" s="6"/>
+      <c r="BS28" s="7"/>
+      <c r="BT28" s="8"/>
       <c r="BU28" s="1"/>
-      <c r="BV28" s="6" t="e">
-        <f>AVERAGE(BV4:BV26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BW28" s="6" t="e">
-        <f>AVERAGE(BW4:BW25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BZ28" s="6" t="e">
-        <f>AVERAGE(BZ4:BZ25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="BX28" s="6"/>
+      <c r="BY28" s="6"/>
+      <c r="CA28" s="7"/>
+      <c r="CB28" s="8"/>
       <c r="CC28" s="1"/>
-      <c r="CD28" s="6" t="e">
-        <f>AVERAGE(CD4:CD26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="CE28" s="6" t="e">
-        <f>AVERAGE(CE4:CE25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="CH28" s="6" t="e">
-        <f>AVERAGE(CH4:CH25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="CF28" s="6"/>
+      <c r="CG28" s="6"/>
+      <c r="CI28" s="7"/>
+      <c r="CJ28" s="8"/>
       <c r="CK28" s="1"/>
-      <c r="CL28" s="6" t="e">
-        <f>AVERAGE(CL4:CL26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="CM28" s="6" t="e">
-        <f>AVERAGE(CM4:CM25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="CP28" s="6" t="e">
-        <f>AVERAGE(CP4:CP25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="CN28" s="6"/>
+      <c r="CO28" s="6"/>
+      <c r="CQ28" s="7"/>
+      <c r="CR28" s="8"/>
       <c r="CS28" s="1"/>
-      <c r="CT28" s="6" t="e">
-        <f>AVERAGE(CT4:CT26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="CU28" s="6" t="e">
-        <f>AVERAGE(CU4:CU25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="CX28" s="6" t="e">
-        <f>AVERAGE(CX4:CX25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="CV28" s="6"/>
+      <c r="CW28" s="6"/>
+      <c r="CY28" s="7"/>
+      <c r="CZ28" s="8"/>
       <c r="DA28" s="1"/>
-      <c r="DB28" s="6" t="e">
-        <f>AVERAGE(DB4:DB26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="DC28" s="6" t="e">
-        <f>AVERAGE(DC4:DC25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="DF28" s="6" t="e">
-        <f>AVERAGE(DF4:DF25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="DD28" s="6"/>
+      <c r="DE28" s="6"/>
+      <c r="DG28" s="7"/>
+      <c r="DH28" s="8"/>
       <c r="DI28" s="1"/>
-      <c r="DJ28" s="6" t="e">
-        <f>AVERAGE(DJ4:DJ26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="DK28" s="6" t="e">
-        <f>AVERAGE(DK4:DK25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="DN28" s="6" t="e">
-        <f>AVERAGE(DN4:DN25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="DL28" s="6"/>
+      <c r="DM28" s="6"/>
+      <c r="DO28" s="7"/>
+      <c r="DP28" s="8"/>
       <c r="DQ28" s="1"/>
-      <c r="DR28" s="6" t="e">
-        <f>AVERAGE(DR4:DR26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="DS28" s="6" t="e">
-        <f>AVERAGE(DS4:DS25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="DV28" s="6" t="e">
-        <f>AVERAGE(DV4:DV25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="DT28" s="6"/>
+      <c r="DU28" s="6"/>
+      <c r="DW28" s="7"/>
+      <c r="DX28" s="8"/>
       <c r="DY28" s="1"/>
-      <c r="DZ28" s="6" t="e">
-        <f>AVERAGE(DZ4:DZ26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="EA28" s="6" t="e">
-        <f>AVERAGE(EA4:EA25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="ED28" s="6" t="e">
-        <f>AVERAGE(ED4:ED25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="EB28" s="6"/>
+      <c r="EC28" s="6"/>
+      <c r="EE28" s="7"/>
+      <c r="EF28" s="8"/>
       <c r="EG28" s="1"/>
-      <c r="EH28" s="6" t="e">
-        <f>AVERAGE(EH4:EH26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="EI28" s="6" t="e">
-        <f>AVERAGE(EI4:EI25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="EL28" s="6" t="e">
-        <f>AVERAGE(EL4:EL25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="EJ28" s="6"/>
+      <c r="EK28" s="6"/>
+      <c r="EM28" s="7"/>
+      <c r="EN28" s="8"/>
       <c r="EO28" s="1"/>
-      <c r="EP28" s="6" t="e">
-        <f>AVERAGE(EP4:EP26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="EQ28" s="6" t="e">
-        <f>AVERAGE(EQ4:EQ25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="ET28" s="6" t="e">
-        <f>AVERAGE(ET4:ET25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="ER28" s="6"/>
+      <c r="ES28" s="6"/>
+      <c r="EU28" s="7"/>
+      <c r="EV28" s="8"/>
       <c r="EW28" s="1"/>
-      <c r="EX28" s="6" t="e">
-        <f>AVERAGE(EX4:EX26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="EY28" s="6" t="e">
-        <f>AVERAGE(EY4:EY25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="FB28" s="6" t="e">
-        <f>AVERAGE(FB4:FB25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="EZ28" s="6"/>
+      <c r="FA28" s="6"/>
+      <c r="FC28" s="7"/>
+      <c r="FD28" s="8"/>
       <c r="FE28" s="1"/>
-      <c r="FF28" s="6" t="e">
-        <f>AVERAGE(FF4:FF26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="FG28" s="6" t="e">
-        <f>AVERAGE(FG4:FG25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="FJ28" s="6" t="e">
-        <f>AVERAGE(FJ4:FJ25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="FH28" s="6"/>
+      <c r="FI28" s="6"/>
+      <c r="FK28" s="7"/>
+      <c r="FL28" s="8"/>
       <c r="FM28" s="1"/>
-      <c r="FN28" s="6" t="e">
-        <f>AVERAGE(FN4:FN26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="FO28" s="6" t="e">
-        <f>AVERAGE(FO4:FO25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="FR28" s="6" t="e">
-        <f>AVERAGE(FR4:FR25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="FP28" s="6"/>
+      <c r="FQ28" s="6"/>
+      <c r="FS28" s="7"/>
+      <c r="FT28" s="8"/>
       <c r="FU28" s="1"/>
     </row>
     <row r="29" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="D29" s="6">
-        <f>SUM(D4:D25)</f>
-        <v>0</v>
-      </c>
+      <c r="A29" s="5"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="8"/>
       <c r="I29" s="1"/>
-      <c r="K29" s="6" t="e">
-        <f>AVERAGE(K4:K28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L29" s="6">
-        <f>SUM(L3:L24)</f>
-        <v>0</v>
-      </c>
+      <c r="L29" s="6"/>
       <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="8"/>
       <c r="Q29" s="1"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6">
-        <f>SUM(T3:T24)</f>
-        <v>0</v>
-      </c>
+      <c r="T29" s="6"/>
       <c r="U29" s="6"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="8"/>
       <c r="Y29" s="1"/>
-      <c r="AA29" s="6"/>
-      <c r="AB29" s="6">
-        <f>SUM(AB3:AB24)</f>
-        <v>0</v>
-      </c>
+      <c r="AB29" s="6"/>
       <c r="AC29" s="6"/>
+      <c r="AE29" s="7"/>
+      <c r="AF29" s="8"/>
       <c r="AG29" s="1"/>
-      <c r="AI29" s="6"/>
-      <c r="AJ29" s="6">
-        <f>SUM(AJ3:AJ24)</f>
-        <v>0</v>
-      </c>
+      <c r="AJ29" s="6"/>
       <c r="AK29" s="6"/>
+      <c r="AM29" s="7"/>
+      <c r="AN29" s="8"/>
       <c r="AO29" s="1"/>
-      <c r="AQ29" s="6"/>
-      <c r="AR29" s="6">
-        <f>SUM(AR3:AR24)</f>
-        <v>0</v>
-      </c>
+      <c r="AR29" s="6"/>
       <c r="AS29" s="6"/>
+      <c r="AU29" s="7"/>
+      <c r="AV29" s="8"/>
       <c r="AW29" s="1"/>
-      <c r="AZ29" s="6">
-        <f>SUM(AZ3:AZ24)</f>
-        <v>0</v>
-      </c>
+      <c r="AX29" s="6"/>
+      <c r="AY29" s="6"/>
+      <c r="AZ29" s="6"/>
+      <c r="BA29" s="6"/>
+      <c r="BB29" s="6"/>
+      <c r="BC29" s="7"/>
+      <c r="BD29" s="8"/>
       <c r="BE29" s="1"/>
-      <c r="BG29" s="6"/>
-      <c r="BH29" s="6">
-        <f>SUM(BH3:BH24)</f>
-        <v>0</v>
-      </c>
+      <c r="BH29" s="6"/>
       <c r="BI29" s="6"/>
+      <c r="BK29" s="7"/>
+      <c r="BL29" s="8"/>
       <c r="BM29" s="1"/>
-      <c r="BO29" s="6"/>
-      <c r="BP29" s="6">
-        <f>SUM(BP3:BP24)</f>
-        <v>0</v>
-      </c>
+      <c r="BP29" s="6"/>
       <c r="BQ29" s="6"/>
+      <c r="BS29" s="7"/>
+      <c r="BT29" s="8"/>
       <c r="BU29" s="1"/>
-      <c r="BW29" s="6"/>
-      <c r="BX29" s="6">
-        <f>SUM(BX3:BX24)</f>
-        <v>0</v>
-      </c>
+      <c r="BX29" s="6"/>
       <c r="BY29" s="6"/>
+      <c r="CA29" s="7"/>
+      <c r="CB29" s="8"/>
       <c r="CC29" s="1"/>
-      <c r="CE29" s="6"/>
-      <c r="CF29" s="6">
-        <f>SUM(CF3:CF24)</f>
-        <v>0</v>
-      </c>
+      <c r="CF29" s="6"/>
       <c r="CG29" s="6"/>
+      <c r="CI29" s="7"/>
+      <c r="CJ29" s="8"/>
       <c r="CK29" s="1"/>
-      <c r="CM29" s="6"/>
-      <c r="CN29" s="6">
-        <f>SUM(CN3:CN24)</f>
-        <v>0</v>
-      </c>
+      <c r="CN29" s="6"/>
       <c r="CO29" s="6"/>
+      <c r="CQ29" s="7"/>
+      <c r="CR29" s="8"/>
       <c r="CS29" s="1"/>
-      <c r="CU29" s="6"/>
-      <c r="CV29" s="6">
-        <f>SUM(CV3:CV24)</f>
-        <v>0</v>
-      </c>
+      <c r="CV29" s="6"/>
       <c r="CW29" s="6"/>
+      <c r="CY29" s="7"/>
+      <c r="CZ29" s="8"/>
       <c r="DA29" s="1"/>
-      <c r="DC29" s="6"/>
-      <c r="DD29" s="6">
-        <f>SUM(DD3:DD24)</f>
-        <v>0</v>
-      </c>
+      <c r="DD29" s="6"/>
       <c r="DE29" s="6"/>
+      <c r="DG29" s="7"/>
+      <c r="DH29" s="8"/>
       <c r="DI29" s="1"/>
-      <c r="DK29" s="6"/>
-      <c r="DL29" s="6">
-        <f>SUM(DL3:DL24)</f>
-        <v>0</v>
-      </c>
+      <c r="DL29" s="6"/>
       <c r="DM29" s="6"/>
+      <c r="DO29" s="7"/>
+      <c r="DP29" s="8"/>
       <c r="DQ29" s="1"/>
-      <c r="DS29" s="6"/>
-      <c r="DT29" s="6">
-        <f>SUM(DT3:DT24)</f>
-        <v>0</v>
-      </c>
+      <c r="DT29" s="6"/>
       <c r="DU29" s="6"/>
+      <c r="DW29" s="7"/>
+      <c r="DX29" s="8"/>
       <c r="DY29" s="1"/>
-      <c r="EA29" s="6"/>
-      <c r="EB29" s="6">
-        <f>SUM(EB3:EB24)</f>
-        <v>0</v>
-      </c>
+      <c r="EB29" s="6"/>
       <c r="EC29" s="6"/>
+      <c r="EE29" s="7"/>
+      <c r="EF29" s="8"/>
       <c r="EG29" s="1"/>
-      <c r="EI29" s="6"/>
-      <c r="EJ29" s="6">
-        <f>SUM(EJ3:EJ24)</f>
-        <v>0</v>
-      </c>
+      <c r="EJ29" s="6"/>
       <c r="EK29" s="6"/>
+      <c r="EM29" s="7"/>
+      <c r="EN29" s="8"/>
       <c r="EO29" s="1"/>
-      <c r="EQ29" s="6"/>
-      <c r="ER29" s="6">
-        <f>SUM(ER3:ER24)</f>
-        <v>0</v>
-      </c>
+      <c r="ER29" s="6"/>
       <c r="ES29" s="6"/>
+      <c r="EU29" s="7"/>
+      <c r="EV29" s="8"/>
       <c r="EW29" s="1"/>
-      <c r="EY29" s="6"/>
-      <c r="EZ29" s="6">
-        <f>SUM(EZ3:EZ24)</f>
-        <v>0</v>
-      </c>
+      <c r="EZ29" s="6"/>
       <c r="FA29" s="6"/>
+      <c r="FC29" s="7"/>
+      <c r="FD29" s="8"/>
       <c r="FE29" s="1"/>
-      <c r="FG29" s="6"/>
-      <c r="FH29" s="6">
-        <f>SUM(FH3:FH24)</f>
-        <v>0</v>
-      </c>
+      <c r="FH29" s="6"/>
       <c r="FI29" s="6"/>
+      <c r="FK29" s="7"/>
+      <c r="FL29" s="8"/>
       <c r="FM29" s="1"/>
-      <c r="FO29" s="6"/>
-      <c r="FP29" s="6">
-        <f>SUM(FP3:FP24)</f>
-        <v>0</v>
-      </c>
+      <c r="FP29" s="6"/>
       <c r="FQ29" s="6"/>
+      <c r="FS29" s="7"/>
+      <c r="FT29" s="8"/>
       <c r="FU29" s="1"/>
     </row>
     <row r="30" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="E30" s="6">
-        <f>SUM(E4:E25)</f>
-        <v>0</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B30" s="27">
+        <f>AVERAGE(B4:B27)</f>
+        <v>311300</v>
+      </c>
+      <c r="C30" s="6" t="e">
+        <f>AVERAGE(C4:C27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F30" s="6" t="e">
+        <f>AVERAGE(F4:F27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G30" s="6"/>
       <c r="I30" s="1"/>
-      <c r="K30" s="6"/>
-      <c r="M30" s="6">
-        <f>SUM(M4:M25)</f>
-        <v>0</v>
-      </c>
-      <c r="N30" s="6"/>
+      <c r="J30" s="6" t="e">
+        <f>AVERAGE(J4:J27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N30" s="6" t="e">
+        <f>AVERAGE(N4:N27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="Q30" s="1"/>
-      <c r="S30" s="6"/>
-      <c r="U30" s="6">
-        <f>SUM(U4:U25)</f>
-        <v>0</v>
-      </c>
-      <c r="V30" s="6"/>
+      <c r="R30" s="6" t="e">
+        <f>AVERAGE(R4:R28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S30" s="6" t="e">
+        <f>AVERAGE(S4:S28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V30" s="6" t="e">
+        <f>AVERAGE(V4:V27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="Y30" s="1"/>
-      <c r="AA30" s="6"/>
-      <c r="AC30" s="6">
-        <f>SUM(AC4:AC25)</f>
-        <v>0</v>
-      </c>
-      <c r="AD30" s="6"/>
+      <c r="Z30" s="6" t="e">
+        <f>AVERAGE(Z4:Z28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA30" s="6" t="e">
+        <f>AVERAGE(AA4:AA27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD30" s="6" t="e">
+        <f>AVERAGE(AD4:AD27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="AG30" s="1"/>
-      <c r="AI30" s="6"/>
-      <c r="AK30" s="6">
-        <f>SUM(AK4:AK25)</f>
-        <v>0</v>
-      </c>
-      <c r="AL30" s="6"/>
+      <c r="AH30" s="6" t="e">
+        <f>AVERAGE(AH4:AH28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI30" s="6" t="e">
+        <f>AVERAGE(AI4:AI27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL30" s="6" t="e">
+        <f>AVERAGE(AL4:AL27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="AO30" s="1"/>
-      <c r="AQ30" s="6"/>
-      <c r="AS30" s="6">
-        <f>SUM(AS4:AS25)</f>
-        <v>0</v>
-      </c>
-      <c r="AT30" s="6"/>
+      <c r="AP30" s="6" t="e">
+        <f>AVERAGE(AP4:AP28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AQ30" s="6" t="e">
+        <f>AVERAGE(AQ4:AQ27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AT30" s="6" t="e">
+        <f>AVERAGE(AT4:AT27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="AW30" s="1"/>
-      <c r="BA30" s="6">
-        <f>SUM(BA4:BA25)</f>
-        <v>0</v>
+      <c r="AX30" s="6" t="e">
+        <f>AVERAGE(AX4:AX28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AY30" s="6" t="e">
+        <f>AVERAGE(AY4:AY27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BB30" s="6" t="e">
+        <f>AVERAGE(BB4:BB27)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="BE30" s="1"/>
-      <c r="BG30" s="6"/>
-      <c r="BI30" s="6">
-        <f>SUM(BI4:BI25)</f>
-        <v>0</v>
-      </c>
-      <c r="BJ30" s="6"/>
+      <c r="BF30" s="6" t="e">
+        <f>AVERAGE(BF4:BF28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BG30" s="6" t="e">
+        <f>AVERAGE(BG4:BG27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BJ30" s="6" t="e">
+        <f>AVERAGE(BJ4:BJ27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="BM30" s="1"/>
-      <c r="BO30" s="6"/>
-      <c r="BQ30" s="6">
-        <f>SUM(BP4:BP25)</f>
-        <v>0</v>
-      </c>
-      <c r="BR30" s="6"/>
+      <c r="BN30" s="6" t="e">
+        <f>AVERAGE(BN4:BN28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BO30" s="6" t="e">
+        <f>AVERAGE(BO4:BO27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BR30" s="6" t="e">
+        <f>AVERAGE(BR4:BR27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="BU30" s="1"/>
-      <c r="BW30" s="6"/>
-      <c r="BY30" s="6">
-        <f>SUM(BY4:BY25)</f>
-        <v>0</v>
-      </c>
-      <c r="BZ30" s="6"/>
+      <c r="BV30" s="6" t="e">
+        <f>AVERAGE(BV4:BV28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BW30" s="6" t="e">
+        <f>AVERAGE(BW4:BW27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BZ30" s="6" t="e">
+        <f>AVERAGE(BZ4:BZ27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="CC30" s="1"/>
-      <c r="CE30" s="6"/>
-      <c r="CG30" s="6">
-        <f>SUM(CG4:CG25)</f>
-        <v>0</v>
-      </c>
-      <c r="CH30" s="6"/>
+      <c r="CD30" s="6" t="e">
+        <f>AVERAGE(CD4:CD28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="CE30" s="6" t="e">
+        <f>AVERAGE(CE4:CE27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="CH30" s="6" t="e">
+        <f>AVERAGE(CH4:CH27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="CK30" s="1"/>
-      <c r="CM30" s="6"/>
-      <c r="CO30" s="6">
-        <f>SUM(CO4:CO25)</f>
-        <v>0</v>
-      </c>
-      <c r="CP30" s="6"/>
+      <c r="CL30" s="6" t="e">
+        <f>AVERAGE(CL4:CL28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="CM30" s="6" t="e">
+        <f>AVERAGE(CM4:CM27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="CP30" s="6" t="e">
+        <f>AVERAGE(CP4:CP27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="CS30" s="1"/>
-      <c r="CU30" s="6"/>
-      <c r="CW30" s="6">
-        <f>SUM(CW4:CW25)</f>
-        <v>0</v>
-      </c>
-      <c r="CX30" s="6"/>
+      <c r="CT30" s="6" t="e">
+        <f>AVERAGE(CT4:CT28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="CU30" s="6" t="e">
+        <f>AVERAGE(CU4:CU27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="CX30" s="6" t="e">
+        <f>AVERAGE(CX4:CX27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="DA30" s="1"/>
-      <c r="DC30" s="6"/>
-      <c r="DE30" s="6">
-        <f>SUM(DE4:DE25)</f>
-        <v>0</v>
-      </c>
-      <c r="DF30" s="6"/>
+      <c r="DB30" s="6" t="e">
+        <f>AVERAGE(DB4:DB28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="DC30" s="6" t="e">
+        <f>AVERAGE(DC4:DC27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="DF30" s="6" t="e">
+        <f>AVERAGE(DF4:DF27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="DI30" s="1"/>
-      <c r="DK30" s="6"/>
-      <c r="DM30" s="6">
-        <f>SUM(DM4:DM25)</f>
-        <v>0</v>
-      </c>
-      <c r="DN30" s="6"/>
+      <c r="DJ30" s="6" t="e">
+        <f>AVERAGE(DJ4:DJ28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="DK30" s="6" t="e">
+        <f>AVERAGE(DK4:DK27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="DN30" s="6" t="e">
+        <f>AVERAGE(DN4:DN27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="DQ30" s="1"/>
-      <c r="DS30" s="6"/>
-      <c r="DU30" s="6">
-        <f>SUM(DU4:DU25)</f>
-        <v>0</v>
-      </c>
-      <c r="DV30" s="6"/>
+      <c r="DR30" s="6" t="e">
+        <f>AVERAGE(DR4:DR28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="DS30" s="6" t="e">
+        <f>AVERAGE(DS4:DS27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="DV30" s="6" t="e">
+        <f>AVERAGE(DV4:DV27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="DY30" s="1"/>
-      <c r="EA30" s="6"/>
-      <c r="EC30" s="6">
-        <f>SUM(EC4:EC25)</f>
-        <v>0</v>
-      </c>
-      <c r="ED30" s="6"/>
+      <c r="DZ30" s="6" t="e">
+        <f>AVERAGE(DZ4:DZ28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="EA30" s="6" t="e">
+        <f>AVERAGE(EA4:EA27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="ED30" s="6" t="e">
+        <f>AVERAGE(ED4:ED27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="EG30" s="1"/>
-      <c r="EI30" s="6"/>
-      <c r="EK30" s="6">
-        <f>SUM(EK4:EK25)</f>
-        <v>0</v>
-      </c>
-      <c r="EL30" s="6"/>
+      <c r="EH30" s="6" t="e">
+        <f>AVERAGE(EH4:EH28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="EI30" s="6" t="e">
+        <f>AVERAGE(EI4:EI27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="EL30" s="6" t="e">
+        <f>AVERAGE(EL4:EL27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="EO30" s="1"/>
-      <c r="EQ30" s="6"/>
-      <c r="ES30" s="6">
-        <f>SUM(ES4:ES25)</f>
-        <v>0</v>
-      </c>
-      <c r="ET30" s="6"/>
+      <c r="EP30" s="6" t="e">
+        <f>AVERAGE(EP4:EP28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="EQ30" s="6" t="e">
+        <f>AVERAGE(EQ4:EQ27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="ET30" s="6" t="e">
+        <f>AVERAGE(ET4:ET27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="EW30" s="1"/>
-      <c r="EY30" s="6"/>
-      <c r="FA30" s="6">
-        <f>SUM(FA4:FA25)</f>
-        <v>0</v>
-      </c>
-      <c r="FB30" s="6"/>
+      <c r="EX30" s="6" t="e">
+        <f>AVERAGE(EX4:EX28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="EY30" s="6" t="e">
+        <f>AVERAGE(EY4:EY27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="FB30" s="6" t="e">
+        <f>AVERAGE(FB4:FB27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="FE30" s="1"/>
-      <c r="FG30" s="6"/>
-      <c r="FI30" s="6">
-        <f>SUM(FI4:FI25)</f>
-        <v>0</v>
-      </c>
-      <c r="FJ30" s="6"/>
+      <c r="FF30" s="6" t="e">
+        <f>AVERAGE(FF4:FF28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="FG30" s="6" t="e">
+        <f>AVERAGE(FG4:FG27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="FJ30" s="6" t="e">
+        <f>AVERAGE(FJ4:FJ27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="FM30" s="1"/>
-      <c r="FO30" s="6"/>
-      <c r="FQ30" s="6">
-        <f>SUM(FQ4:FQ25)</f>
-        <v>0</v>
-      </c>
-      <c r="FR30" s="6"/>
+      <c r="FN30" s="6" t="e">
+        <f>AVERAGE(FN4:FN28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="FO30" s="6" t="e">
+        <f>AVERAGE(FO4:FO27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="FR30" s="6" t="e">
+        <f>AVERAGE(FR4:FR27)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="FU30" s="1"/>
     </row>
     <row r="31" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="H31" s="10">
-        <f>SUM(H4:H25)</f>
+      <c r="D31" s="6">
+        <f>SUM(D4:D27)</f>
         <v>0</v>
       </c>
       <c r="I31" s="1"/>
-      <c r="N31" s="6"/>
-      <c r="P31" s="10">
-        <f>SUM(P4:P25)</f>
+      <c r="K31" s="6" t="e">
+        <f>AVERAGE(K4:K30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L31" s="6">
+        <f>SUM(L3:L26)</f>
         <v>0</v>
       </c>
+      <c r="M31" s="6"/>
       <c r="Q31" s="1"/>
-      <c r="V31" s="6"/>
-      <c r="X31" s="10">
-        <f>SUM(X4:X25)</f>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6">
+        <f>SUM(T3:T26)</f>
         <v>0</v>
       </c>
+      <c r="U31" s="6"/>
       <c r="Y31" s="1"/>
-      <c r="AD31" s="6"/>
-      <c r="AF31" s="10">
-        <f>SUM(AF4:AF25)</f>
+      <c r="AA31" s="6"/>
+      <c r="AB31" s="6">
+        <f>SUM(AB3:AB26)</f>
         <v>0</v>
       </c>
+      <c r="AC31" s="6"/>
       <c r="AG31" s="1"/>
-      <c r="AL31" s="6"/>
-      <c r="AN31" s="10">
-        <f>SUM(AN4:AN25)</f>
+      <c r="AI31" s="6"/>
+      <c r="AJ31" s="6">
+        <f>SUM(AJ3:AJ26)</f>
         <v>0</v>
       </c>
+      <c r="AK31" s="6"/>
       <c r="AO31" s="1"/>
-      <c r="AT31" s="6"/>
-      <c r="AV31" s="10">
-        <f>SUM(AV4:AV25)</f>
+      <c r="AQ31" s="6"/>
+      <c r="AR31" s="6">
+        <f>SUM(AR3:AR26)</f>
         <v>0</v>
       </c>
+      <c r="AS31" s="6"/>
       <c r="AW31" s="1"/>
-      <c r="BB31" s="6"/>
-      <c r="BD31" s="10">
-        <f>SUM(BD4:BD25)</f>
+      <c r="AZ31" s="6">
+        <f>SUM(AZ3:AZ26)</f>
         <v>0</v>
       </c>
       <c r="BE31" s="1"/>
-      <c r="BJ31" s="6"/>
-      <c r="BL31" s="10">
-        <f>SUM(BL4:BL25)</f>
+      <c r="BG31" s="6"/>
+      <c r="BH31" s="6">
+        <f>SUM(BH3:BH26)</f>
         <v>0</v>
       </c>
+      <c r="BI31" s="6"/>
       <c r="BM31" s="1"/>
-      <c r="BR31" s="6"/>
-      <c r="BT31" s="10">
-        <f>SUM(BT4:BT25)</f>
+      <c r="BO31" s="6"/>
+      <c r="BP31" s="6">
+        <f>SUM(BP3:BP26)</f>
         <v>0</v>
       </c>
+      <c r="BQ31" s="6"/>
       <c r="BU31" s="1"/>
-      <c r="BZ31" s="6"/>
+      <c r="BW31" s="6"/>
+      <c r="BX31" s="6">
+        <f>SUM(BX3:BX26)</f>
+        <v>0</v>
+      </c>
+      <c r="BY31" s="6"/>
       <c r="CC31" s="1"/>
-      <c r="CH31" s="6"/>
-      <c r="CJ31" s="10">
-        <f>SUM(CJ4:CJ25)</f>
+      <c r="CE31" s="6"/>
+      <c r="CF31" s="6">
+        <f>SUM(CF3:CF26)</f>
         <v>0</v>
       </c>
+      <c r="CG31" s="6"/>
       <c r="CK31" s="1"/>
-      <c r="CP31" s="6"/>
-      <c r="CR31" s="10">
-        <f>SUM(CR4:CR25)</f>
+      <c r="CM31" s="6"/>
+      <c r="CN31" s="6">
+        <f>SUM(CN3:CN26)</f>
         <v>0</v>
       </c>
+      <c r="CO31" s="6"/>
       <c r="CS31" s="1"/>
-      <c r="CX31" s="6"/>
-      <c r="CZ31" s="10">
-        <f>SUM(CZ4:CZ25)</f>
+      <c r="CU31" s="6"/>
+      <c r="CV31" s="6">
+        <f>SUM(CV3:CV26)</f>
         <v>0</v>
       </c>
+      <c r="CW31" s="6"/>
       <c r="DA31" s="1"/>
-      <c r="DF31" s="6"/>
-      <c r="DH31" s="10">
-        <f>SUM(DH4:DH25)</f>
+      <c r="DC31" s="6"/>
+      <c r="DD31" s="6">
+        <f>SUM(DD3:DD26)</f>
         <v>0</v>
       </c>
+      <c r="DE31" s="6"/>
       <c r="DI31" s="1"/>
-      <c r="DN31" s="6"/>
-      <c r="DP31" s="10">
-        <f>SUM(DP4:DP25)</f>
+      <c r="DK31" s="6"/>
+      <c r="DL31" s="6">
+        <f>SUM(DL3:DL26)</f>
         <v>0</v>
       </c>
+      <c r="DM31" s="6"/>
       <c r="DQ31" s="1"/>
-      <c r="DV31" s="6"/>
-      <c r="DX31" s="10">
-        <f>SUM(DX4:DX25)</f>
+      <c r="DS31" s="6"/>
+      <c r="DT31" s="6">
+        <f>SUM(DT3:DT26)</f>
         <v>0</v>
       </c>
+      <c r="DU31" s="6"/>
       <c r="DY31" s="1"/>
-      <c r="ED31" s="6"/>
-      <c r="EF31" s="10">
-        <f>SUM(EF4:EF25)</f>
+      <c r="EA31" s="6"/>
+      <c r="EB31" s="6">
+        <f>SUM(EB3:EB26)</f>
         <v>0</v>
       </c>
+      <c r="EC31" s="6"/>
       <c r="EG31" s="1"/>
-      <c r="EL31" s="6"/>
-      <c r="EN31" s="10">
-        <f>SUM(EN4:EN25)</f>
+      <c r="EI31" s="6"/>
+      <c r="EJ31" s="6">
+        <f>SUM(EJ3:EJ26)</f>
         <v>0</v>
       </c>
+      <c r="EK31" s="6"/>
       <c r="EO31" s="1"/>
-      <c r="ET31" s="6"/>
-      <c r="EV31" s="10">
-        <f>SUM(EV4:EV25)</f>
+      <c r="EQ31" s="6"/>
+      <c r="ER31" s="6">
+        <f>SUM(ER3:ER26)</f>
         <v>0</v>
       </c>
+      <c r="ES31" s="6"/>
       <c r="EW31" s="1"/>
-      <c r="FB31" s="6"/>
-      <c r="FD31" s="10">
-        <f>SUM(FD4:FD25)</f>
+      <c r="EY31" s="6"/>
+      <c r="EZ31" s="6">
+        <f>SUM(EZ3:EZ26)</f>
         <v>0</v>
       </c>
+      <c r="FA31" s="6"/>
       <c r="FE31" s="1"/>
-      <c r="FJ31" s="6"/>
-      <c r="FL31" s="10">
-        <f>SUM(FL4:FL25)</f>
+      <c r="FG31" s="6"/>
+      <c r="FH31" s="6">
+        <f>SUM(FH3:FH26)</f>
         <v>0</v>
       </c>
+      <c r="FI31" s="6"/>
       <c r="FM31" s="1"/>
-      <c r="FR31" s="6"/>
-      <c r="FT31" s="10">
-        <f>SUM(FT4:FT25)</f>
+      <c r="FO31" s="6"/>
+      <c r="FP31" s="6">
+        <f>SUM(FP3:FP26)</f>
         <v>0</v>
       </c>
+      <c r="FQ31" s="6"/>
       <c r="FU31" s="1"/>
     </row>
     <row r="32" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="E32" s="6">
+        <f>SUM(E4:E27)</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="K32" s="6"/>
+      <c r="M32" s="6">
+        <f>SUM(M4:M27)</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="6"/>
+      <c r="Q32" s="1"/>
+      <c r="S32" s="6"/>
+      <c r="U32" s="6">
+        <f>SUM(U4:U27)</f>
+        <v>0</v>
+      </c>
+      <c r="V32" s="6"/>
+      <c r="Y32" s="1"/>
+      <c r="AA32" s="6"/>
+      <c r="AC32" s="6">
+        <f>SUM(AC4:AC27)</f>
+        <v>0</v>
+      </c>
+      <c r="AD32" s="6"/>
+      <c r="AG32" s="1"/>
+      <c r="AI32" s="6"/>
+      <c r="AK32" s="6">
+        <f>SUM(AK4:AK27)</f>
+        <v>0</v>
+      </c>
+      <c r="AL32" s="6"/>
+      <c r="AO32" s="1"/>
+      <c r="AQ32" s="6"/>
+      <c r="AS32" s="6">
+        <f>SUM(AS4:AS27)</f>
+        <v>0</v>
+      </c>
+      <c r="AT32" s="6"/>
+      <c r="AW32" s="1"/>
+      <c r="BA32" s="6">
+        <f>SUM(BA4:BA27)</f>
+        <v>0</v>
+      </c>
+      <c r="BE32" s="1"/>
+      <c r="BG32" s="6"/>
+      <c r="BI32" s="6">
+        <f>SUM(BI4:BI27)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ32" s="6"/>
+      <c r="BM32" s="1"/>
+      <c r="BO32" s="6"/>
+      <c r="BQ32" s="6">
+        <f>SUM(BP4:BP27)</f>
+        <v>0</v>
+      </c>
+      <c r="BR32" s="6"/>
+      <c r="BU32" s="1"/>
+      <c r="BW32" s="6"/>
+      <c r="BY32" s="6">
+        <f>SUM(BY4:BY27)</f>
+        <v>0</v>
+      </c>
+      <c r="BZ32" s="6"/>
+      <c r="CC32" s="1"/>
+      <c r="CE32" s="6"/>
+      <c r="CG32" s="6">
+        <f>SUM(CG4:CG27)</f>
+        <v>0</v>
+      </c>
+      <c r="CH32" s="6"/>
+      <c r="CK32" s="1"/>
+      <c r="CM32" s="6"/>
+      <c r="CO32" s="6">
+        <f>SUM(CO4:CO27)</f>
+        <v>0</v>
+      </c>
+      <c r="CP32" s="6"/>
+      <c r="CS32" s="1"/>
+      <c r="CU32" s="6"/>
+      <c r="CW32" s="6">
+        <f>SUM(CW4:CW27)</f>
+        <v>0</v>
+      </c>
+      <c r="CX32" s="6"/>
+      <c r="DA32" s="1"/>
+      <c r="DC32" s="6"/>
+      <c r="DE32" s="6">
+        <f>SUM(DE4:DE27)</f>
+        <v>0</v>
+      </c>
+      <c r="DF32" s="6"/>
+      <c r="DI32" s="1"/>
+      <c r="DK32" s="6"/>
+      <c r="DM32" s="6">
+        <f>SUM(DM4:DM27)</f>
+        <v>0</v>
+      </c>
+      <c r="DN32" s="6"/>
+      <c r="DQ32" s="1"/>
+      <c r="DS32" s="6"/>
+      <c r="DU32" s="6">
+        <f>SUM(DU4:DU27)</f>
+        <v>0</v>
+      </c>
+      <c r="DV32" s="6"/>
+      <c r="DY32" s="1"/>
+      <c r="EA32" s="6"/>
+      <c r="EC32" s="6">
+        <f>SUM(EC4:EC27)</f>
+        <v>0</v>
+      </c>
+      <c r="ED32" s="6"/>
+      <c r="EG32" s="1"/>
+      <c r="EI32" s="6"/>
+      <c r="EK32" s="6">
+        <f>SUM(EK4:EK27)</f>
+        <v>0</v>
+      </c>
+      <c r="EL32" s="6"/>
+      <c r="EO32" s="1"/>
+      <c r="EQ32" s="6"/>
+      <c r="ES32" s="6">
+        <f>SUM(ES4:ES27)</f>
+        <v>0</v>
+      </c>
+      <c r="ET32" s="6"/>
+      <c r="EW32" s="1"/>
+      <c r="EY32" s="6"/>
+      <c r="FA32" s="6">
+        <f>SUM(FA4:FA27)</f>
+        <v>0</v>
+      </c>
+      <c r="FB32" s="6"/>
+      <c r="FE32" s="1"/>
+      <c r="FG32" s="6"/>
+      <c r="FI32" s="6">
+        <f>SUM(FI4:FI27)</f>
+        <v>0</v>
+      </c>
+      <c r="FJ32" s="6"/>
+      <c r="FM32" s="1"/>
+      <c r="FO32" s="6"/>
+      <c r="FQ32" s="6">
+        <f>SUM(FQ4:FQ27)</f>
+        <v>0</v>
+      </c>
+      <c r="FR32" s="6"/>
+      <c r="FU32" s="1"/>
+    </row>
+    <row r="33" spans="1:177" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="H33" s="10">
+        <f>SUM(H4:H27)</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="1"/>
+      <c r="N33" s="6"/>
+      <c r="P33" s="10">
+        <f>SUM(P4:P27)</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1"/>
+      <c r="V33" s="6"/>
+      <c r="X33" s="10">
+        <f>SUM(X4:X27)</f>
+        <v>0</v>
+      </c>
+      <c r="Y33" s="1"/>
+      <c r="AD33" s="6"/>
+      <c r="AF33" s="10">
+        <f>SUM(AF4:AF27)</f>
+        <v>0</v>
+      </c>
+      <c r="AG33" s="1"/>
+      <c r="AL33" s="6"/>
+      <c r="AN33" s="10">
+        <f>SUM(AN4:AN27)</f>
+        <v>0</v>
+      </c>
+      <c r="AO33" s="1"/>
+      <c r="AT33" s="6"/>
+      <c r="AV33" s="10">
+        <f>SUM(AV4:AV27)</f>
+        <v>0</v>
+      </c>
+      <c r="AW33" s="1"/>
+      <c r="BB33" s="6"/>
+      <c r="BD33" s="10">
+        <f>SUM(BD4:BD27)</f>
+        <v>0</v>
+      </c>
+      <c r="BE33" s="1"/>
+      <c r="BJ33" s="6"/>
+      <c r="BL33" s="10">
+        <f>SUM(BL4:BL27)</f>
+        <v>0</v>
+      </c>
+      <c r="BM33" s="1"/>
+      <c r="BR33" s="6"/>
+      <c r="BT33" s="10">
+        <f>SUM(BT4:BT27)</f>
+        <v>0</v>
+      </c>
+      <c r="BU33" s="1"/>
+      <c r="BZ33" s="6"/>
+      <c r="CC33" s="1"/>
+      <c r="CH33" s="6"/>
+      <c r="CJ33" s="10">
+        <f>SUM(CJ4:CJ27)</f>
+        <v>0</v>
+      </c>
+      <c r="CK33" s="1"/>
+      <c r="CP33" s="6"/>
+      <c r="CR33" s="10">
+        <f>SUM(CR4:CR27)</f>
+        <v>0</v>
+      </c>
+      <c r="CS33" s="1"/>
+      <c r="CX33" s="6"/>
+      <c r="CZ33" s="10">
+        <f>SUM(CZ4:CZ27)</f>
+        <v>0</v>
+      </c>
+      <c r="DA33" s="1"/>
+      <c r="DF33" s="6"/>
+      <c r="DH33" s="10">
+        <f>SUM(DH4:DH27)</f>
+        <v>0</v>
+      </c>
+      <c r="DI33" s="1"/>
+      <c r="DN33" s="6"/>
+      <c r="DP33" s="10">
+        <f>SUM(DP4:DP27)</f>
+        <v>0</v>
+      </c>
+      <c r="DQ33" s="1"/>
+      <c r="DV33" s="6"/>
+      <c r="DX33" s="10">
+        <f>SUM(DX4:DX27)</f>
+        <v>0</v>
+      </c>
+      <c r="DY33" s="1"/>
+      <c r="ED33" s="6"/>
+      <c r="EF33" s="10">
+        <f>SUM(EF4:EF27)</f>
+        <v>0</v>
+      </c>
+      <c r="EG33" s="1"/>
+      <c r="EL33" s="6"/>
+      <c r="EN33" s="10">
+        <f>SUM(EN4:EN27)</f>
+        <v>0</v>
+      </c>
+      <c r="EO33" s="1"/>
+      <c r="ET33" s="6"/>
+      <c r="EV33" s="10">
+        <f>SUM(EV4:EV27)</f>
+        <v>0</v>
+      </c>
+      <c r="EW33" s="1"/>
+      <c r="FB33" s="6"/>
+      <c r="FD33" s="10">
+        <f>SUM(FD4:FD27)</f>
+        <v>0</v>
+      </c>
+      <c r="FE33" s="1"/>
+      <c r="FJ33" s="6"/>
+      <c r="FL33" s="10">
+        <f>SUM(FL4:FL27)</f>
+        <v>0</v>
+      </c>
+      <c r="FM33" s="1"/>
+      <c r="FR33" s="6"/>
+      <c r="FT33" s="10">
+        <f>SUM(FT4:FT27)</f>
+        <v>0</v>
+      </c>
+      <c r="FU33" s="1"/>
+    </row>
+    <row r="34" spans="1:177" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="H32" s="10">
+      <c r="B34" s="6"/>
+      <c r="H34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="I32" s="1"/>
-      <c r="P32" s="10">
+      <c r="I34" s="1"/>
+      <c r="P34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="Q32" s="1"/>
-      <c r="X32" s="10">
+      <c r="Q34" s="1"/>
+      <c r="X34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="Y32" s="1"/>
-      <c r="AF32" s="10">
+      <c r="Y34" s="1"/>
+      <c r="AF34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="AG32" s="1"/>
-      <c r="AN32" s="10">
+      <c r="AG34" s="1"/>
+      <c r="AN34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="AO32" s="1"/>
-      <c r="AV32" s="10">
+      <c r="AO34" s="1"/>
+      <c r="AV34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="AW32" s="1"/>
-      <c r="BD32" s="10">
+      <c r="AW34" s="1"/>
+      <c r="BD34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="BE32" s="1"/>
-      <c r="BL32" s="10">
+      <c r="BE34" s="1"/>
+      <c r="BL34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="BM32" s="1"/>
-      <c r="BT32" s="10">
+      <c r="BM34" s="1"/>
+      <c r="BT34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="BU32" s="1"/>
-      <c r="CC32" s="1"/>
-      <c r="CJ32" s="10">
+      <c r="BU34" s="1"/>
+      <c r="CC34" s="1"/>
+      <c r="CJ34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="CK32" s="1"/>
-      <c r="CR32" s="10">
+      <c r="CK34" s="1"/>
+      <c r="CR34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="CS32" s="1"/>
-      <c r="CZ32" s="10">
+      <c r="CS34" s="1"/>
+      <c r="CZ34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="DA32" s="1"/>
-      <c r="DH32" s="10">
+      <c r="DA34" s="1"/>
+      <c r="DH34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="DI32" s="1"/>
-      <c r="DP32" s="10">
+      <c r="DI34" s="1"/>
+      <c r="DP34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="DQ32" s="1"/>
-      <c r="DX32" s="10">
+      <c r="DQ34" s="1"/>
+      <c r="DX34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="DY32" s="1"/>
-      <c r="EF32" s="10">
+      <c r="DY34" s="1"/>
+      <c r="EF34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="EG32" s="1"/>
-      <c r="EN32" s="10">
+      <c r="EG34" s="1"/>
+      <c r="EN34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="EO32" s="1"/>
-      <c r="EV32" s="10">
+      <c r="EO34" s="1"/>
+      <c r="EV34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="EW32" s="1"/>
-      <c r="FD32" s="10">
+      <c r="EW34" s="1"/>
+      <c r="FD34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="FE32" s="1"/>
-      <c r="FL32" s="10">
+      <c r="FE34" s="1"/>
+      <c r="FL34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="FM32" s="1"/>
-      <c r="FT32" s="10">
+      <c r="FM34" s="1"/>
+      <c r="FT34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
-      <c r="FU32" s="1"/>
+      <c r="FU34" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+    <row r="36" spans="1:177" x14ac:dyDescent="0.2">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="39" spans="1:177" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="40" spans="1:177" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="41" spans="1:177" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="BF1:CB1"/>
+    <mergeCell ref="CD1:DP1"/>
+    <mergeCell ref="DR1:EF1"/>
+    <mergeCell ref="DZ2:EF2"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="CT2:CZ2"/>
+    <mergeCell ref="DB2:DH2"/>
+    <mergeCell ref="DJ2:DP2"/>
+    <mergeCell ref="AX2:BD2"/>
+    <mergeCell ref="BF2:BK2"/>
+    <mergeCell ref="BN2:BT2"/>
+    <mergeCell ref="EX1:FD1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="CL2:CR2"/>
+    <mergeCell ref="DR2:DX2"/>
+    <mergeCell ref="EH1:EV1"/>
     <mergeCell ref="FF1:FL1"/>
     <mergeCell ref="BV2:CB2"/>
     <mergeCell ref="FN1:FT1"/>
@@ -6231,27 +7049,10 @@
     <mergeCell ref="FN2:FT2"/>
     <mergeCell ref="CD2:CJ2"/>
     <mergeCell ref="EH2:EN2"/>
-    <mergeCell ref="EX1:FD1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="CL2:CR2"/>
-    <mergeCell ref="DR2:DX2"/>
-    <mergeCell ref="EH1:EV1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="BF1:CB1"/>
-    <mergeCell ref="CD1:DP1"/>
-    <mergeCell ref="DR1:EF1"/>
-    <mergeCell ref="DZ2:EF2"/>
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="CT2:CZ2"/>
-    <mergeCell ref="DB2:DH2"/>
-    <mergeCell ref="DJ2:DP2"/>
-    <mergeCell ref="AX2:BD2"/>
-    <mergeCell ref="BF2:BK2"/>
-    <mergeCell ref="BN2:BT2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
-      <formula>$F$6&gt;$F$28 + $F$28*0.2</formula>
+  <conditionalFormatting sqref="F6:F7">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+      <formula>$F$6&gt;$F$30 + $F$30*0.2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cap nhat du lieu hom nay va ngay 29/11 cho ma VND
</commit_message>
<xml_diff>
--- a/2023/Demo.xlsx
+++ b/2023/Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trung.nguyenhoang/Documents/github/2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6114083D-9C0E-CF4D-885A-3211C16D5FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE4B345-1254-B640-8B22-BD32AF54E5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17080" xr2:uid="{B7EC2610-802E-D441-AB46-76A27057AA52}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="96">
   <si>
     <t>CHỨNG KHOÁN</t>
   </si>
@@ -315,6 +315,18 @@
   </si>
   <si>
     <t>2.82%</t>
+  </si>
+  <si>
+    <t>9.46%</t>
+  </si>
+  <si>
+    <t>4.13%</t>
+  </si>
+  <si>
+    <t>10.61%</t>
+  </si>
+  <si>
+    <t>1.20%</t>
   </si>
 </sst>
 </file>
@@ -512,6 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -557,7 +570,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,13 +611,7 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="36">
-          <cell r="D36">
-            <v>1.1999999999999971E-3</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -910,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9267E568-C429-F945-A885-A15FECEEE65C}">
   <dimension ref="A1:FU41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C12" sqref="C12"/>
     </sheetView>
@@ -935,431 +941,431 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
+      <c r="B1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="16" t="s">
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="16"/>
+      <c r="AN1" s="16"/>
+      <c r="AO1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="AP1" s="16"/>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="16"/>
-      <c r="AT1" s="16"/>
-      <c r="AU1" s="16"/>
-      <c r="AV1" s="16"/>
-      <c r="AW1" s="16"/>
-      <c r="AX1" s="16"/>
-      <c r="AY1" s="16"/>
-      <c r="AZ1" s="16"/>
-      <c r="BA1" s="16"/>
-      <c r="BB1" s="16"/>
-      <c r="BC1" s="16"/>
+      <c r="AP1" s="17"/>
+      <c r="AQ1" s="17"/>
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17"/>
+      <c r="AV1" s="17"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
+      <c r="AY1" s="17"/>
+      <c r="AZ1" s="17"/>
+      <c r="BA1" s="17"/>
+      <c r="BB1" s="17"/>
+      <c r="BC1" s="17"/>
       <c r="BD1" s="1"/>
       <c r="BE1" s="1"/>
-      <c r="BF1" s="21" t="s">
+      <c r="BF1" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="BG1" s="21"/>
-      <c r="BH1" s="21"/>
-      <c r="BI1" s="21"/>
-      <c r="BJ1" s="21"/>
-      <c r="BK1" s="21"/>
-      <c r="BL1" s="21"/>
-      <c r="BM1" s="21"/>
-      <c r="BN1" s="21"/>
-      <c r="BO1" s="21"/>
-      <c r="BP1" s="21"/>
-      <c r="BQ1" s="21"/>
-      <c r="BR1" s="21"/>
-      <c r="BS1" s="21"/>
-      <c r="BT1" s="21"/>
-      <c r="BU1" s="21"/>
-      <c r="BV1" s="21"/>
-      <c r="BW1" s="21"/>
-      <c r="BX1" s="21"/>
-      <c r="BY1" s="21"/>
-      <c r="BZ1" s="21"/>
-      <c r="CA1" s="21"/>
-      <c r="CB1" s="21"/>
+      <c r="BG1" s="22"/>
+      <c r="BH1" s="22"/>
+      <c r="BI1" s="22"/>
+      <c r="BJ1" s="22"/>
+      <c r="BK1" s="22"/>
+      <c r="BL1" s="22"/>
+      <c r="BM1" s="22"/>
+      <c r="BN1" s="22"/>
+      <c r="BO1" s="22"/>
+      <c r="BP1" s="22"/>
+      <c r="BQ1" s="22"/>
+      <c r="BR1" s="22"/>
+      <c r="BS1" s="22"/>
+      <c r="BT1" s="22"/>
+      <c r="BU1" s="22"/>
+      <c r="BV1" s="22"/>
+      <c r="BW1" s="22"/>
+      <c r="BX1" s="22"/>
+      <c r="BY1" s="22"/>
+      <c r="BZ1" s="22"/>
+      <c r="CA1" s="22"/>
+      <c r="CB1" s="22"/>
       <c r="CC1" s="1"/>
-      <c r="CD1" s="22" t="s">
+      <c r="CD1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="CE1" s="22"/>
-      <c r="CF1" s="22"/>
-      <c r="CG1" s="22"/>
-      <c r="CH1" s="22"/>
-      <c r="CI1" s="22"/>
-      <c r="CJ1" s="22"/>
-      <c r="CK1" s="22"/>
-      <c r="CL1" s="22"/>
-      <c r="CM1" s="22"/>
-      <c r="CN1" s="22"/>
-      <c r="CO1" s="22"/>
-      <c r="CP1" s="22"/>
-      <c r="CQ1" s="22"/>
-      <c r="CR1" s="22"/>
-      <c r="CS1" s="22"/>
-      <c r="CT1" s="22"/>
-      <c r="CU1" s="22"/>
-      <c r="CV1" s="22"/>
-      <c r="CW1" s="22"/>
-      <c r="CX1" s="22"/>
-      <c r="CY1" s="22"/>
-      <c r="CZ1" s="22"/>
-      <c r="DA1" s="22"/>
-      <c r="DB1" s="22"/>
-      <c r="DC1" s="22"/>
-      <c r="DD1" s="22"/>
-      <c r="DE1" s="22"/>
-      <c r="DF1" s="22"/>
-      <c r="DG1" s="22"/>
-      <c r="DH1" s="22"/>
-      <c r="DI1" s="22"/>
-      <c r="DJ1" s="22"/>
-      <c r="DK1" s="22"/>
-      <c r="DL1" s="22"/>
-      <c r="DM1" s="22"/>
-      <c r="DN1" s="22"/>
-      <c r="DO1" s="22"/>
-      <c r="DP1" s="22"/>
+      <c r="CE1" s="23"/>
+      <c r="CF1" s="23"/>
+      <c r="CG1" s="23"/>
+      <c r="CH1" s="23"/>
+      <c r="CI1" s="23"/>
+      <c r="CJ1" s="23"/>
+      <c r="CK1" s="23"/>
+      <c r="CL1" s="23"/>
+      <c r="CM1" s="23"/>
+      <c r="CN1" s="23"/>
+      <c r="CO1" s="23"/>
+      <c r="CP1" s="23"/>
+      <c r="CQ1" s="23"/>
+      <c r="CR1" s="23"/>
+      <c r="CS1" s="23"/>
+      <c r="CT1" s="23"/>
+      <c r="CU1" s="23"/>
+      <c r="CV1" s="23"/>
+      <c r="CW1" s="23"/>
+      <c r="CX1" s="23"/>
+      <c r="CY1" s="23"/>
+      <c r="CZ1" s="23"/>
+      <c r="DA1" s="23"/>
+      <c r="DB1" s="23"/>
+      <c r="DC1" s="23"/>
+      <c r="DD1" s="23"/>
+      <c r="DE1" s="23"/>
+      <c r="DF1" s="23"/>
+      <c r="DG1" s="23"/>
+      <c r="DH1" s="23"/>
+      <c r="DI1" s="23"/>
+      <c r="DJ1" s="23"/>
+      <c r="DK1" s="23"/>
+      <c r="DL1" s="23"/>
+      <c r="DM1" s="23"/>
+      <c r="DN1" s="23"/>
+      <c r="DO1" s="23"/>
+      <c r="DP1" s="23"/>
       <c r="DQ1" s="1"/>
-      <c r="DR1" s="23" t="s">
+      <c r="DR1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="DS1" s="23"/>
-      <c r="DT1" s="23"/>
-      <c r="DU1" s="23"/>
-      <c r="DV1" s="23"/>
-      <c r="DW1" s="23"/>
-      <c r="DX1" s="23"/>
-      <c r="DY1" s="23"/>
-      <c r="DZ1" s="23"/>
-      <c r="EA1" s="23"/>
-      <c r="EB1" s="23"/>
-      <c r="EC1" s="23"/>
-      <c r="ED1" s="23"/>
-      <c r="EE1" s="23"/>
-      <c r="EF1" s="23"/>
+      <c r="DS1" s="24"/>
+      <c r="DT1" s="24"/>
+      <c r="DU1" s="24"/>
+      <c r="DV1" s="24"/>
+      <c r="DW1" s="24"/>
+      <c r="DX1" s="24"/>
+      <c r="DY1" s="24"/>
+      <c r="DZ1" s="24"/>
+      <c r="EA1" s="24"/>
+      <c r="EB1" s="24"/>
+      <c r="EC1" s="24"/>
+      <c r="ED1" s="24"/>
+      <c r="EE1" s="24"/>
+      <c r="EF1" s="24"/>
       <c r="EG1" s="1"/>
-      <c r="EH1" s="19" t="s">
+      <c r="EH1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="EI1" s="19"/>
-      <c r="EJ1" s="19"/>
-      <c r="EK1" s="19"/>
-      <c r="EL1" s="19"/>
-      <c r="EM1" s="19"/>
-      <c r="EN1" s="19"/>
-      <c r="EO1" s="19"/>
-      <c r="EP1" s="19"/>
-      <c r="EQ1" s="19"/>
-      <c r="ER1" s="19"/>
-      <c r="ES1" s="19"/>
-      <c r="ET1" s="19"/>
-      <c r="EU1" s="19"/>
-      <c r="EV1" s="19"/>
+      <c r="EI1" s="20"/>
+      <c r="EJ1" s="20"/>
+      <c r="EK1" s="20"/>
+      <c r="EL1" s="20"/>
+      <c r="EM1" s="20"/>
+      <c r="EN1" s="20"/>
+      <c r="EO1" s="20"/>
+      <c r="EP1" s="20"/>
+      <c r="EQ1" s="20"/>
+      <c r="ER1" s="20"/>
+      <c r="ES1" s="20"/>
+      <c r="ET1" s="20"/>
+      <c r="EU1" s="20"/>
+      <c r="EV1" s="20"/>
       <c r="EW1" s="1"/>
-      <c r="EX1" s="17" t="s">
+      <c r="EX1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="EY1" s="17"/>
-      <c r="EZ1" s="17"/>
-      <c r="FA1" s="17"/>
-      <c r="FB1" s="17"/>
-      <c r="FC1" s="17"/>
-      <c r="FD1" s="17"/>
+      <c r="EY1" s="18"/>
+      <c r="EZ1" s="18"/>
+      <c r="FA1" s="18"/>
+      <c r="FB1" s="18"/>
+      <c r="FC1" s="18"/>
+      <c r="FD1" s="18"/>
       <c r="FE1" s="1"/>
-      <c r="FF1" s="12" t="s">
+      <c r="FF1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="FG1" s="12"/>
-      <c r="FH1" s="12"/>
-      <c r="FI1" s="12"/>
-      <c r="FJ1" s="12"/>
-      <c r="FK1" s="12"/>
-      <c r="FL1" s="12"/>
+      <c r="FG1" s="13"/>
+      <c r="FH1" s="13"/>
+      <c r="FI1" s="13"/>
+      <c r="FJ1" s="13"/>
+      <c r="FK1" s="13"/>
+      <c r="FL1" s="13"/>
       <c r="FM1" s="1"/>
-      <c r="FN1" s="14" t="s">
+      <c r="FN1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="FO1" s="14"/>
-      <c r="FP1" s="14"/>
-      <c r="FQ1" s="14"/>
-      <c r="FR1" s="14"/>
-      <c r="FS1" s="14"/>
-      <c r="FT1" s="14"/>
+      <c r="FO1" s="15"/>
+      <c r="FP1" s="15"/>
+      <c r="FQ1" s="15"/>
+      <c r="FR1" s="15"/>
+      <c r="FS1" s="15"/>
+      <c r="FT1" s="15"/>
       <c r="FU1" s="1"/>
     </row>
     <row r="2" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A2" s="20"/>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="21"/>
+      <c r="B2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="13" t="s">
+      <c r="Z2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="13"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
       <c r="AG2" s="1"/>
-      <c r="AH2" s="13" t="s">
+      <c r="AH2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="13"/>
-      <c r="AK2" s="13"/>
-      <c r="AL2" s="13"/>
-      <c r="AM2" s="13"/>
-      <c r="AN2" s="13"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="14"/>
       <c r="AO2" s="1"/>
-      <c r="AP2" s="13" t="s">
+      <c r="AP2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AQ2" s="13"/>
-      <c r="AR2" s="13"/>
-      <c r="AS2" s="13"/>
-      <c r="AT2" s="13"/>
-      <c r="AU2" s="13"/>
-      <c r="AV2" s="13"/>
+      <c r="AQ2" s="14"/>
+      <c r="AR2" s="14"/>
+      <c r="AS2" s="14"/>
+      <c r="AT2" s="14"/>
+      <c r="AU2" s="14"/>
+      <c r="AV2" s="14"/>
       <c r="AW2" s="1"/>
-      <c r="AX2" s="25" t="s">
+      <c r="AX2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="AY2" s="25"/>
-      <c r="AZ2" s="25"/>
-      <c r="BA2" s="25"/>
-      <c r="BB2" s="25"/>
-      <c r="BC2" s="25"/>
-      <c r="BD2" s="26"/>
+      <c r="AY2" s="26"/>
+      <c r="AZ2" s="26"/>
+      <c r="BA2" s="26"/>
+      <c r="BB2" s="26"/>
+      <c r="BC2" s="26"/>
+      <c r="BD2" s="27"/>
       <c r="BE2" s="1"/>
-      <c r="BF2" s="25" t="s">
+      <c r="BF2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="BG2" s="25"/>
-      <c r="BH2" s="25"/>
-      <c r="BI2" s="25"/>
-      <c r="BJ2" s="25"/>
-      <c r="BK2" s="26"/>
+      <c r="BG2" s="26"/>
+      <c r="BH2" s="26"/>
+      <c r="BI2" s="26"/>
+      <c r="BJ2" s="26"/>
+      <c r="BK2" s="27"/>
       <c r="BL2" s="2"/>
       <c r="BM2" s="1"/>
-      <c r="BN2" s="13" t="s">
+      <c r="BN2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="BO2" s="13"/>
-      <c r="BP2" s="13"/>
-      <c r="BQ2" s="13"/>
-      <c r="BR2" s="13"/>
-      <c r="BS2" s="13"/>
-      <c r="BT2" s="13"/>
+      <c r="BO2" s="14"/>
+      <c r="BP2" s="14"/>
+      <c r="BQ2" s="14"/>
+      <c r="BR2" s="14"/>
+      <c r="BS2" s="14"/>
+      <c r="BT2" s="14"/>
       <c r="BU2" s="1"/>
-      <c r="BV2" s="13" t="s">
+      <c r="BV2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="BW2" s="13"/>
-      <c r="BX2" s="13"/>
-      <c r="BY2" s="13"/>
-      <c r="BZ2" s="13"/>
-      <c r="CA2" s="13"/>
-      <c r="CB2" s="13"/>
+      <c r="BW2" s="14"/>
+      <c r="BX2" s="14"/>
+      <c r="BY2" s="14"/>
+      <c r="BZ2" s="14"/>
+      <c r="CA2" s="14"/>
+      <c r="CB2" s="14"/>
       <c r="CC2" s="1"/>
-      <c r="CD2" s="13" t="s">
+      <c r="CD2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="CE2" s="13"/>
-      <c r="CF2" s="13"/>
-      <c r="CG2" s="13"/>
-      <c r="CH2" s="13"/>
-      <c r="CI2" s="13"/>
-      <c r="CJ2" s="13"/>
+      <c r="CE2" s="14"/>
+      <c r="CF2" s="14"/>
+      <c r="CG2" s="14"/>
+      <c r="CH2" s="14"/>
+      <c r="CI2" s="14"/>
+      <c r="CJ2" s="14"/>
       <c r="CK2" s="1"/>
-      <c r="CL2" s="13" t="s">
+      <c r="CL2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="CM2" s="13"/>
-      <c r="CN2" s="13"/>
-      <c r="CO2" s="13"/>
-      <c r="CP2" s="13"/>
-      <c r="CQ2" s="13"/>
-      <c r="CR2" s="13"/>
+      <c r="CM2" s="14"/>
+      <c r="CN2" s="14"/>
+      <c r="CO2" s="14"/>
+      <c r="CP2" s="14"/>
+      <c r="CQ2" s="14"/>
+      <c r="CR2" s="14"/>
       <c r="CS2" s="1"/>
-      <c r="CT2" s="13" t="s">
+      <c r="CT2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="CU2" s="13"/>
-      <c r="CV2" s="13"/>
-      <c r="CW2" s="13"/>
-      <c r="CX2" s="13"/>
-      <c r="CY2" s="13"/>
-      <c r="CZ2" s="13"/>
+      <c r="CU2" s="14"/>
+      <c r="CV2" s="14"/>
+      <c r="CW2" s="14"/>
+      <c r="CX2" s="14"/>
+      <c r="CY2" s="14"/>
+      <c r="CZ2" s="14"/>
       <c r="DA2" s="1"/>
-      <c r="DB2" s="13" t="s">
+      <c r="DB2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="DC2" s="13"/>
-      <c r="DD2" s="13"/>
-      <c r="DE2" s="13"/>
-      <c r="DF2" s="13"/>
-      <c r="DG2" s="13"/>
-      <c r="DH2" s="13"/>
+      <c r="DC2" s="14"/>
+      <c r="DD2" s="14"/>
+      <c r="DE2" s="14"/>
+      <c r="DF2" s="14"/>
+      <c r="DG2" s="14"/>
+      <c r="DH2" s="14"/>
       <c r="DI2" s="1"/>
-      <c r="DJ2" s="13" t="s">
+      <c r="DJ2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="DK2" s="13"/>
-      <c r="DL2" s="13"/>
-      <c r="DM2" s="13"/>
-      <c r="DN2" s="13"/>
-      <c r="DO2" s="13"/>
-      <c r="DP2" s="13"/>
+      <c r="DK2" s="14"/>
+      <c r="DL2" s="14"/>
+      <c r="DM2" s="14"/>
+      <c r="DN2" s="14"/>
+      <c r="DO2" s="14"/>
+      <c r="DP2" s="14"/>
       <c r="DQ2" s="1"/>
-      <c r="DR2" s="13" t="s">
+      <c r="DR2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="DS2" s="13"/>
-      <c r="DT2" s="13"/>
-      <c r="DU2" s="13"/>
-      <c r="DV2" s="13"/>
-      <c r="DW2" s="13"/>
-      <c r="DX2" s="13"/>
+      <c r="DS2" s="14"/>
+      <c r="DT2" s="14"/>
+      <c r="DU2" s="14"/>
+      <c r="DV2" s="14"/>
+      <c r="DW2" s="14"/>
+      <c r="DX2" s="14"/>
       <c r="DY2" s="1"/>
-      <c r="DZ2" s="13" t="s">
+      <c r="DZ2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="EA2" s="13"/>
-      <c r="EB2" s="13"/>
-      <c r="EC2" s="13"/>
-      <c r="ED2" s="13"/>
-      <c r="EE2" s="13"/>
-      <c r="EF2" s="13"/>
+      <c r="EA2" s="14"/>
+      <c r="EB2" s="14"/>
+      <c r="EC2" s="14"/>
+      <c r="ED2" s="14"/>
+      <c r="EE2" s="14"/>
+      <c r="EF2" s="14"/>
       <c r="EG2" s="1"/>
-      <c r="EH2" s="13" t="s">
+      <c r="EH2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="EI2" s="13"/>
-      <c r="EJ2" s="13"/>
-      <c r="EK2" s="13"/>
-      <c r="EL2" s="13"/>
-      <c r="EM2" s="13"/>
-      <c r="EN2" s="13"/>
+      <c r="EI2" s="14"/>
+      <c r="EJ2" s="14"/>
+      <c r="EK2" s="14"/>
+      <c r="EL2" s="14"/>
+      <c r="EM2" s="14"/>
+      <c r="EN2" s="14"/>
       <c r="EO2" s="1"/>
-      <c r="EP2" s="13" t="s">
+      <c r="EP2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="EQ2" s="13"/>
-      <c r="ER2" s="13"/>
-      <c r="ES2" s="13"/>
-      <c r="ET2" s="13"/>
-      <c r="EU2" s="13"/>
-      <c r="EV2" s="13"/>
+      <c r="EQ2" s="14"/>
+      <c r="ER2" s="14"/>
+      <c r="ES2" s="14"/>
+      <c r="ET2" s="14"/>
+      <c r="EU2" s="14"/>
+      <c r="EV2" s="14"/>
       <c r="EW2" s="1"/>
-      <c r="EX2" s="13" t="s">
+      <c r="EX2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="EY2" s="13"/>
-      <c r="EZ2" s="13"/>
-      <c r="FA2" s="13"/>
-      <c r="FB2" s="13"/>
-      <c r="FC2" s="13"/>
-      <c r="FD2" s="13"/>
+      <c r="EY2" s="14"/>
+      <c r="EZ2" s="14"/>
+      <c r="FA2" s="14"/>
+      <c r="FB2" s="14"/>
+      <c r="FC2" s="14"/>
+      <c r="FD2" s="14"/>
       <c r="FE2" s="1"/>
-      <c r="FF2" s="13" t="s">
+      <c r="FF2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="FG2" s="13"/>
-      <c r="FH2" s="13"/>
-      <c r="FI2" s="13"/>
-      <c r="FJ2" s="13"/>
-      <c r="FK2" s="13"/>
-      <c r="FL2" s="13"/>
+      <c r="FG2" s="14"/>
+      <c r="FH2" s="14"/>
+      <c r="FI2" s="14"/>
+      <c r="FJ2" s="14"/>
+      <c r="FK2" s="14"/>
+      <c r="FL2" s="14"/>
       <c r="FM2" s="1"/>
-      <c r="FN2" s="13" t="s">
+      <c r="FN2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="FO2" s="13"/>
-      <c r="FP2" s="13"/>
-      <c r="FQ2" s="13"/>
-      <c r="FR2" s="13"/>
-      <c r="FS2" s="13"/>
-      <c r="FT2" s="13"/>
+      <c r="FO2" s="14"/>
+      <c r="FP2" s="14"/>
+      <c r="FQ2" s="14"/>
+      <c r="FR2" s="14"/>
+      <c r="FS2" s="14"/>
+      <c r="FT2" s="14"/>
       <c r="FU2" s="1"/>
     </row>
     <row r="3" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="11" t="s">
         <v>32</v>
       </c>
@@ -4328,13 +4334,27 @@
       <c r="A16" s="5">
         <v>45259</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="8"/>
+      <c r="B16" s="6">
+        <v>1580515</v>
+      </c>
+      <c r="C16" s="6">
+        <v>276500</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1304015</v>
+      </c>
+      <c r="E16" s="6">
+        <v>27424930000</v>
+      </c>
+      <c r="F16" s="6">
+        <v>17510500</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -4870,8 +4890,27 @@
       <c r="A19" s="5">
         <v>45264</v>
       </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="8"/>
+      <c r="B19">
+        <v>538084</v>
+      </c>
+      <c r="C19">
+        <v>4817210</v>
+      </c>
+      <c r="D19">
+        <v>-4279126</v>
+      </c>
+      <c r="E19">
+        <v>-95296010000</v>
+      </c>
+      <c r="F19">
+        <v>56592100</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>93</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
@@ -6146,7 +6185,7 @@
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="27">
+      <c r="B30" s="12">
         <f>AVERAGE(B4:B27)</f>
         <v>311300</v>
       </c>
@@ -6887,108 +6926,108 @@
       <c r="B34" s="6"/>
       <c r="H34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="I34" s="1"/>
       <c r="P34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="1"/>
       <c r="X34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="Y34" s="1"/>
       <c r="AF34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="AG34" s="1"/>
       <c r="AN34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="AO34" s="1"/>
       <c r="AV34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="AW34" s="1"/>
       <c r="BD34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="BE34" s="1"/>
       <c r="BL34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="BM34" s="1"/>
       <c r="BT34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="BU34" s="1"/>
       <c r="CC34" s="1"/>
       <c r="CJ34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="CK34" s="1"/>
       <c r="CR34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="CS34" s="1"/>
       <c r="CZ34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="DA34" s="1"/>
       <c r="DH34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="DI34" s="1"/>
       <c r="DP34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="DQ34" s="1"/>
       <c r="DX34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="DY34" s="1"/>
       <c r="EF34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="EG34" s="1"/>
       <c r="EN34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="EO34" s="1"/>
       <c r="EV34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="EW34" s="1"/>
       <c r="FD34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="FE34" s="1"/>
       <c r="FL34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="FM34" s="1"/>
       <c r="FT34" s="10">
         <f>'[1]VNINDEX T11-T12'!D36</f>
-        <v>1.1999999999999971E-3</v>
+        <v>0</v>
       </c>
       <c r="FU34" s="1"/>
     </row>

</xml_diff>